<commit_message>
run AMD samples on CPU
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -1,12 +1,12 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1850,7 +1850,11 @@
       <c r="J29" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="K29" s="8" t="n"/>
+      <c r="K29" s="8" t="inlineStr">
+        <is>
+          <t>0.0528379000</t>
+        </is>
+      </c>
       <c r="L29" s="8" t="inlineStr">
         <is>
           <t>0.0003475150</t>
@@ -1893,7 +1897,11 @@
       <c r="J30" s="7" t="n">
         <v>4</v>
       </c>
-      <c r="K30" s="8" t="n"/>
+      <c r="K30" s="8" t="inlineStr">
+        <is>
+          <t>0.0140000000</t>
+        </is>
+      </c>
       <c r="L30" s="8" t="inlineStr">
         <is>
           <t>0.0060000000</t>
@@ -1936,7 +1944,11 @@
       <c r="J31" s="7" t="n">
         <v>12</v>
       </c>
-      <c r="K31" s="8" t="n"/>
+      <c r="K31" s="8" t="inlineStr">
+        <is>
+          <t>0.5789000000</t>
+        </is>
+      </c>
       <c r="L31" s="8" t="inlineStr">
         <is>
           <t>0.5760600000</t>
@@ -1979,7 +1991,11 @@
       <c r="J32" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="K32" s="8" t="n"/>
+      <c r="K32" s="8" t="inlineStr">
+        <is>
+          <t>0.4280000000</t>
+        </is>
+      </c>
       <c r="L32" s="8" t="inlineStr">
         <is>
           <t>0.1030000000</t>
@@ -2022,7 +2038,11 @@
       <c r="J33" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="K33" s="8" t="n"/>
+      <c r="K33" s="8" t="inlineStr">
+        <is>
+          <t>0.6647100000</t>
+        </is>
+      </c>
       <c r="L33" s="8" t="inlineStr">
         <is>
           <t>0.6865900000</t>
@@ -2065,7 +2085,11 @@
       <c r="J34" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="K34" s="8" t="n"/>
+      <c r="K34" s="8" t="inlineStr">
+        <is>
+          <t>0.6452500000</t>
+        </is>
+      </c>
       <c r="L34" s="8" t="inlineStr">
         <is>
           <t>0.7585000000</t>
@@ -2108,7 +2132,11 @@
       <c r="J35" s="7" t="n">
         <v>8</v>
       </c>
-      <c r="K35" s="8" t="n"/>
+      <c r="K35" s="8" t="inlineStr">
+        <is>
+          <t>0.7257500000</t>
+        </is>
+      </c>
       <c r="L35" s="8" t="inlineStr">
         <is>
           <t>0.7711400000</t>
@@ -2151,7 +2179,11 @@
       <c r="J36" s="7" t="n">
         <v>10</v>
       </c>
-      <c r="K36" s="8" t="n"/>
+      <c r="K36" s="8" t="inlineStr">
+        <is>
+          <t>0.3880000000</t>
+        </is>
+      </c>
       <c r="L36" s="8" t="inlineStr">
         <is>
           <t>0.0110000000</t>
@@ -2194,7 +2226,11 @@
       <c r="J37" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="K37" s="8" t="n"/>
+      <c r="K37" s="8" t="inlineStr">
+        <is>
+          <t>0.6890500000</t>
+        </is>
+      </c>
       <c r="L37" s="8" t="inlineStr">
         <is>
           <t>0.5800300000</t>
@@ -2237,7 +2273,11 @@
       <c r="J38" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="K38" s="8" t="n"/>
+      <c r="K38" s="8" t="inlineStr">
+        <is>
+          <t>0.6660800000</t>
+        </is>
+      </c>
       <c r="L38" s="8" t="inlineStr">
         <is>
           <t>0.6761200000</t>
@@ -2280,7 +2320,11 @@
       <c r="J39" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="K39" s="8" t="n"/>
+      <c r="K39" s="8" t="inlineStr">
+        <is>
+          <t>0.6112400000</t>
+        </is>
+      </c>
       <c r="L39" s="8" t="inlineStr">
         <is>
           <t>0.6751200000</t>
@@ -2323,7 +2367,11 @@
       <c r="J40" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="K40" s="8" t="n"/>
+      <c r="K40" s="8" t="inlineStr">
+        <is>
+          <t>0.6583600000</t>
+        </is>
+      </c>
       <c r="L40" s="8" t="inlineStr">
         <is>
           <t>0.6565700000</t>
@@ -2366,7 +2414,11 @@
       <c r="J41" s="7" t="n">
         <v>2</v>
       </c>
-      <c r="K41" s="8" t="n"/>
+      <c r="K41" s="8" t="inlineStr">
+        <is>
+          <t>0.6252900000</t>
+        </is>
+      </c>
       <c r="L41" s="8" t="inlineStr">
         <is>
           <t>0.5911300000</t>
@@ -2409,7 +2461,11 @@
       <c r="J42" s="7" t="n">
         <v>30</v>
       </c>
-      <c r="K42" s="8" t="n"/>
+      <c r="K42" s="8" t="inlineStr">
+        <is>
+          <t>0.6474900000</t>
+        </is>
+      </c>
       <c r="L42" s="8" t="inlineStr">
         <is>
           <t>0.6041900000</t>
@@ -2452,7 +2508,11 @@
       <c r="J43" s="7" t="n">
         <v>332</v>
       </c>
-      <c r="K43" s="8" t="n"/>
+      <c r="K43" s="8" t="inlineStr">
+        <is>
+          <t>0.6949400000</t>
+        </is>
+      </c>
       <c r="L43" s="8" t="inlineStr">
         <is>
           <t>0.5711200000</t>
@@ -2495,7 +2555,11 @@
       <c r="J44" s="7" t="n">
         <v>128</v>
       </c>
-      <c r="K44" s="8" t="n"/>
+      <c r="K44" s="8" t="inlineStr">
+        <is>
+          <t>0.7830000000</t>
+        </is>
+      </c>
       <c r="L44" s="8" t="inlineStr">
         <is>
           <t>0.5740000000</t>
@@ -2538,7 +2602,11 @@
       <c r="J45" s="7" t="n">
         <v>12</v>
       </c>
-      <c r="K45" s="8" t="n"/>
+      <c r="K45" s="8" t="inlineStr">
+        <is>
+          <t>0.6440800000</t>
+        </is>
+      </c>
       <c r="L45" s="8" t="inlineStr">
         <is>
           <t>0.5640800000</t>
@@ -2581,7 +2649,11 @@
       <c r="J46" s="7" t="n">
         <v>115</v>
       </c>
-      <c r="K46" s="8" t="n"/>
+      <c r="K46" s="8" t="inlineStr">
+        <is>
+          <t>23.4670000000</t>
+        </is>
+      </c>
       <c r="L46" s="8" t="inlineStr">
         <is>
           <t>0.3470000000</t>
@@ -2624,7 +2696,11 @@
       <c r="J47" s="7" t="n">
         <v>84</v>
       </c>
-      <c r="K47" s="8" t="n"/>
+      <c r="K47" s="8" t="inlineStr">
+        <is>
+          <t>1.2809300000</t>
+        </is>
+      </c>
       <c r="L47" s="8" t="inlineStr">
         <is>
           <t>0.7104400000</t>
@@ -2667,7 +2743,11 @@
       <c r="J48" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="K48" s="8" t="n"/>
+      <c r="K48" s="8" t="inlineStr">
+        <is>
+          <t>0.0140000000</t>
+        </is>
+      </c>
       <c r="L48" s="8" t="inlineStr">
         <is>
           <t>0.0020000000</t>
@@ -2710,7 +2790,11 @@
       <c r="J49" s="7" t="n">
         <v>30</v>
       </c>
-      <c r="K49" s="8" t="n"/>
+      <c r="K49" s="8" t="inlineStr">
+        <is>
+          <t>0.0050000000</t>
+        </is>
+      </c>
       <c r="L49" s="8" t="inlineStr">
         <is>
           <t>0.0010000000</t>
@@ -2753,7 +2837,11 @@
       <c r="J50" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="K50" s="8" t="n"/>
+      <c r="K50" s="8" t="inlineStr">
+        <is>
+          <t>0.1110000000</t>
+        </is>
+      </c>
       <c r="L50" s="8" t="inlineStr">
         <is>
           <t>0.0610000000</t>
@@ -2796,7 +2884,11 @@
       <c r="J51" s="7" t="n">
         <v>56</v>
       </c>
-      <c r="K51" s="8" t="n"/>
+      <c r="K51" s="8" t="inlineStr">
+        <is>
+          <t>0.5719000000</t>
+        </is>
+      </c>
       <c r="L51" s="8" t="inlineStr">
         <is>
           <t>0.6849700000</t>
@@ -2839,7 +2931,11 @@
       <c r="J52" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="K52" s="8" t="n"/>
+      <c r="K52" s="8" t="inlineStr">
+        <is>
+          <t>0.6080700000</t>
+        </is>
+      </c>
       <c r="L52" s="8" t="inlineStr">
         <is>
           <t>0.6690400000</t>
@@ -2882,7 +2978,11 @@
       <c r="J53" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="K53" s="8" t="n"/>
+      <c r="K53" s="8" t="inlineStr">
+        <is>
+          <t>0.0130000000</t>
+        </is>
+      </c>
       <c r="L53" s="8" t="inlineStr">
         <is>
           <t>0.0030000000</t>
@@ -2925,7 +3025,11 @@
       <c r="J54" s="7" t="n">
         <v>4</v>
       </c>
-      <c r="K54" s="8" t="n"/>
+      <c r="K54" s="8" t="inlineStr">
+        <is>
+          <t>0.5607500000</t>
+        </is>
+      </c>
       <c r="L54" s="8" t="inlineStr">
         <is>
           <t>0.7050300000</t>
@@ -2968,7 +3072,11 @@
       <c r="J55" s="7" t="n">
         <v>9</v>
       </c>
-      <c r="K55" s="8" t="n"/>
+      <c r="K55" s="8" t="inlineStr">
+        <is>
+          <t>0.5937400000</t>
+        </is>
+      </c>
       <c r="L55" s="8" t="inlineStr">
         <is>
           <t>0.6913200000</t>
@@ -3011,7 +3119,11 @@
       <c r="J56" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="K56" s="8" t="n"/>
+      <c r="K56" s="8" t="inlineStr">
+        <is>
+          <t>0.5751100000</t>
+        </is>
+      </c>
       <c r="L56" s="8" t="inlineStr">
         <is>
           <t>0.6692100000</t>
@@ -3054,7 +3166,11 @@
       <c r="J57" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="K57" s="8" t="n"/>
+      <c r="K57" s="8" t="inlineStr">
+        <is>
+          <t>0.0380000000</t>
+        </is>
+      </c>
       <c r="L57" s="8" t="inlineStr">
         <is>
           <t>0.0240000000</t>
@@ -3097,7 +3213,11 @@
       <c r="J58" s="7" t="n">
         <v>6</v>
       </c>
-      <c r="K58" s="8" t="n"/>
+      <c r="K58" s="8" t="inlineStr">
+        <is>
+          <t>4.3045000000</t>
+        </is>
+      </c>
       <c r="L58" s="8" t="inlineStr">
         <is>
           <t>0.5590070000</t>
@@ -3140,7 +3260,11 @@
       <c r="J59" s="7" t="n">
         <v>5</v>
       </c>
-      <c r="K59" s="8" t="n"/>
+      <c r="K59" s="8" t="inlineStr">
+        <is>
+          <t>0.6114800000</t>
+        </is>
+      </c>
       <c r="L59" s="8" t="inlineStr">
         <is>
           <t>0.6673300000</t>

</xml_diff>

<commit_message>
run rodinia on CPU
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -3307,10 +3307,14 @@
       <c r="J60" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="K60" s="8" t="n"/>
+      <c r="K60" s="8" t="inlineStr">
+        <is>
+          <t>0.0823160000</t>
+        </is>
+      </c>
       <c r="L60" s="8" t="inlineStr">
         <is>
-          <t>1.1023510000</t>
+          <t>0.0975790000</t>
         </is>
       </c>
       <c r="M60" s="7" t="n"/>
@@ -3350,10 +3354,14 @@
       <c r="J61" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="K61" s="8" t="n"/>
+      <c r="K61" s="8" t="inlineStr">
+        <is>
+          <t>0.6391930000</t>
+        </is>
+      </c>
       <c r="L61" s="8" t="inlineStr">
         <is>
-          <t>1.2315690000</t>
+          <t>0.6694910000</t>
         </is>
       </c>
       <c r="M61" s="7" t="n"/>
@@ -3393,10 +3401,14 @@
       <c r="J62" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="K62" s="8" t="n"/>
+      <c r="K62" s="8" t="inlineStr">
+        <is>
+          <t>0.1200500000</t>
+        </is>
+      </c>
       <c r="L62" s="8" t="inlineStr">
         <is>
-          <t>0.8207750000</t>
+          <t>0.7782530000</t>
         </is>
       </c>
       <c r="M62" s="7" t="n"/>
@@ -3436,10 +3448,14 @@
       <c r="J63" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="K63" s="8" t="n"/>
+      <c r="K63" s="8" t="inlineStr">
+        <is>
+          <t>8.6193270000</t>
+        </is>
+      </c>
       <c r="L63" s="8" t="inlineStr">
         <is>
-          <t>2.0738050000</t>
+          <t>8.4539560000</t>
         </is>
       </c>
       <c r="M63" s="7" t="n"/>
@@ -3479,10 +3495,14 @@
       <c r="J64" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="K64" s="8" t="n"/>
+      <c r="K64" s="8" t="inlineStr">
+        <is>
+          <t>0.1033040000</t>
+        </is>
+      </c>
       <c r="L64" s="8" t="inlineStr">
         <is>
-          <t>0.9154540000</t>
+          <t>0.1483920000</t>
         </is>
       </c>
       <c r="M64" s="7" t="n"/>
@@ -3522,10 +3542,14 @@
       <c r="J65" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="K65" s="8" t="n"/>
+      <c r="K65" s="8" t="inlineStr">
+        <is>
+          <t>4.0266510000</t>
+        </is>
+      </c>
       <c r="L65" s="8" t="inlineStr">
         <is>
-          <t>1.2217640000</t>
+          <t>5.4771270000</t>
         </is>
       </c>
       <c r="M65" s="7" t="n"/>
@@ -3565,10 +3589,14 @@
       <c r="J66" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="K66" s="8" t="n"/>
+      <c r="K66" s="8" t="inlineStr">
+        <is>
+          <t>12.3171850000</t>
+        </is>
+      </c>
       <c r="L66" s="8" t="inlineStr">
         <is>
-          <t>1.3119770000</t>
+          <t>12.2726530000</t>
         </is>
       </c>
       <c r="M66" s="7" t="n"/>
@@ -3608,10 +3636,14 @@
       <c r="J67" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="K67" s="8" t="n"/>
+      <c r="K67" s="8" t="inlineStr">
+        <is>
+          <t>32.7613950000</t>
+        </is>
+      </c>
       <c r="L67" s="8" t="inlineStr">
         <is>
-          <t>1.4004680000</t>
+          <t>33.2539140000</t>
         </is>
       </c>
       <c r="M67" s="7" t="n"/>
@@ -3651,10 +3683,14 @@
       <c r="J68" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="K68" s="8" t="n"/>
+      <c r="K68" s="8" t="inlineStr">
+        <is>
+          <t>0.9711030000</t>
+        </is>
+      </c>
       <c r="L68" s="8" t="inlineStr">
         <is>
-          <t>0.2666820000</t>
+          <t>1.6896860000</t>
         </is>
       </c>
       <c r="M68" s="7" t="n"/>
@@ -3694,10 +3730,14 @@
       <c r="J69" s="7" t="n">
         <v>58</v>
       </c>
-      <c r="K69" s="8" t="n"/>
+      <c r="K69" s="8" t="inlineStr">
+        <is>
+          <t>0.2438150000</t>
+        </is>
+      </c>
       <c r="L69" s="8" t="inlineStr">
         <is>
-          <t>0.3303970000</t>
+          <t>0.3204090000</t>
         </is>
       </c>
       <c r="M69" s="7" t="n"/>
@@ -3737,10 +3777,14 @@
       <c r="J70" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="K70" s="8" t="n"/>
+      <c r="K70" s="8" t="inlineStr">
+        <is>
+          <t>31.5730360000</t>
+        </is>
+      </c>
       <c r="L70" s="8" t="inlineStr">
         <is>
-          <t>1.2654730000</t>
+          <t>32.2186160000</t>
         </is>
       </c>
       <c r="M70" s="7" t="n"/>
@@ -3780,10 +3824,14 @@
       <c r="J71" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="K71" s="8" t="n"/>
+      <c r="K71" s="8" t="inlineStr">
+        <is>
+          <t>18.7550030000</t>
+        </is>
+      </c>
       <c r="L71" s="8" t="inlineStr">
         <is>
-          <t>1.1739230000</t>
+          <t>19.6663000000</t>
         </is>
       </c>
       <c r="M71" s="7" t="n"/>
@@ -3823,10 +3871,14 @@
       <c r="J72" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="K72" s="8" t="n"/>
+      <c r="K72" s="8" t="inlineStr">
+        <is>
+          <t>1.7172340000</t>
+        </is>
+      </c>
       <c r="L72" s="8" t="inlineStr">
         <is>
-          <t>3.0554540000</t>
+          <t>1.9030160000</t>
         </is>
       </c>
       <c r="M72" s="7" t="n"/>
@@ -3866,10 +3918,14 @@
       <c r="J73" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="K73" s="8" t="n"/>
+      <c r="K73" s="8" t="inlineStr">
+        <is>
+          <t>0.0606480000</t>
+        </is>
+      </c>
       <c r="L73" s="8" t="inlineStr">
         <is>
-          <t>0.0102400000</t>
+          <t>0.0606480000</t>
         </is>
       </c>
       <c r="M73" s="7" t="n"/>
@@ -3909,10 +3965,14 @@
       <c r="J74" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="K74" s="8" t="n"/>
+      <c r="K74" s="8" t="inlineStr">
+        <is>
+          <t>0.4908550000</t>
+        </is>
+      </c>
       <c r="L74" s="8" t="inlineStr">
         <is>
-          <t>1.0165660000</t>
+          <t>1.5245870000</t>
         </is>
       </c>
       <c r="M74" s="7" t="n"/>
@@ -3952,10 +4012,14 @@
       <c r="J75" s="7" t="n">
         <v>6</v>
       </c>
-      <c r="K75" s="8" t="n"/>
+      <c r="K75" s="8" t="inlineStr">
+        <is>
+          <t>0.4632210000</t>
+        </is>
+      </c>
       <c r="L75" s="8" t="inlineStr">
         <is>
-          <t>1.7146530000</t>
+          <t>1.4709390000</t>
         </is>
       </c>
       <c r="M75" s="7" t="n"/>
@@ -3995,10 +4059,14 @@
       <c r="J76" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="K76" s="8" t="n"/>
+      <c r="K76" s="8" t="inlineStr">
+        <is>
+          <t>0.3353120000</t>
+        </is>
+      </c>
       <c r="L76" s="8" t="inlineStr">
         <is>
-          <t>4.4722670000</t>
+          <t>1.3506390000</t>
         </is>
       </c>
       <c r="M76" s="7" t="n"/>
@@ -4081,10 +4149,14 @@
       <c r="J78" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="K78" s="8" t="n"/>
+      <c r="K78" s="8" t="inlineStr">
+        <is>
+          <t>11.2296740000</t>
+        </is>
+      </c>
       <c r="L78" s="8" t="inlineStr">
         <is>
-          <t>4.2263010000</t>
+          <t>65.7484890000</t>
         </is>
       </c>
       <c r="M78" s="7" t="n"/>
@@ -4124,10 +4196,14 @@
       <c r="J79" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="K79" s="8" t="n"/>
+      <c r="K79" s="8" t="inlineStr">
+        <is>
+          <t>1.1714820000</t>
+        </is>
+      </c>
       <c r="L79" s="8" t="inlineStr">
         <is>
-          <t>1.3099670000</t>
+          <t>1.1548690000</t>
         </is>
       </c>
       <c r="M79" s="7" t="n"/>

</xml_diff>

<commit_message>
run rodinia on GPU
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -1,12 +1,12 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -3314,7 +3314,7 @@
       </c>
       <c r="L60" s="8" t="inlineStr">
         <is>
-          <t>0.0975790000</t>
+          <t>1.1325580000</t>
         </is>
       </c>
       <c r="M60" s="7" t="n"/>
@@ -3361,7 +3361,7 @@
       </c>
       <c r="L61" s="8" t="inlineStr">
         <is>
-          <t>0.6694910000</t>
+          <t>1.2671750000</t>
         </is>
       </c>
       <c r="M61" s="7" t="n"/>
@@ -3408,7 +3408,7 @@
       </c>
       <c r="L62" s="8" t="inlineStr">
         <is>
-          <t>0.7782530000</t>
+          <t>0.8565370000</t>
         </is>
       </c>
       <c r="M62" s="7" t="n"/>
@@ -3455,7 +3455,7 @@
       </c>
       <c r="L63" s="8" t="inlineStr">
         <is>
-          <t>8.4539560000</t>
+          <t>1.9598740000</t>
         </is>
       </c>
       <c r="M63" s="7" t="n"/>
@@ -3502,7 +3502,7 @@
       </c>
       <c r="L64" s="8" t="inlineStr">
         <is>
-          <t>0.1483920000</t>
+          <t>0.8027820000</t>
         </is>
       </c>
       <c r="M64" s="7" t="n"/>
@@ -3549,7 +3549,7 @@
       </c>
       <c r="L65" s="8" t="inlineStr">
         <is>
-          <t>5.4771270000</t>
+          <t>1.1964120000</t>
         </is>
       </c>
       <c r="M65" s="7" t="n"/>
@@ -3596,7 +3596,7 @@
       </c>
       <c r="L66" s="8" t="inlineStr">
         <is>
-          <t>12.2726530000</t>
+          <t>1.2765400000</t>
         </is>
       </c>
       <c r="M66" s="7" t="n"/>
@@ -3643,7 +3643,7 @@
       </c>
       <c r="L67" s="8" t="inlineStr">
         <is>
-          <t>33.2539140000</t>
+          <t>1.3033110000</t>
         </is>
       </c>
       <c r="M67" s="7" t="n"/>
@@ -3690,7 +3690,7 @@
       </c>
       <c r="L68" s="8" t="inlineStr">
         <is>
-          <t>1.6896860000</t>
+          <t>0.2607990000</t>
         </is>
       </c>
       <c r="M68" s="7" t="n"/>
@@ -3737,7 +3737,7 @@
       </c>
       <c r="L69" s="8" t="inlineStr">
         <is>
-          <t>0.3204090000</t>
+          <t>0.3520820000</t>
         </is>
       </c>
       <c r="M69" s="7" t="n"/>
@@ -3784,7 +3784,7 @@
       </c>
       <c r="L70" s="8" t="inlineStr">
         <is>
-          <t>32.2186160000</t>
+          <t>1.3297930000</t>
         </is>
       </c>
       <c r="M70" s="7" t="n"/>
@@ -3831,7 +3831,7 @@
       </c>
       <c r="L71" s="8" t="inlineStr">
         <is>
-          <t>19.6663000000</t>
+          <t>1.2440830000</t>
         </is>
       </c>
       <c r="M71" s="7" t="n"/>
@@ -3878,7 +3878,7 @@
       </c>
       <c r="L72" s="8" t="inlineStr">
         <is>
-          <t>1.9030160000</t>
+          <t>2.9664410000</t>
         </is>
       </c>
       <c r="M72" s="7" t="n"/>
@@ -3925,7 +3925,7 @@
       </c>
       <c r="L73" s="8" t="inlineStr">
         <is>
-          <t>0.0606480000</t>
+          <t>0.0102400000</t>
         </is>
       </c>
       <c r="M73" s="7" t="n"/>
@@ -3972,7 +3972,7 @@
       </c>
       <c r="L74" s="8" t="inlineStr">
         <is>
-          <t>1.5245870000</t>
+          <t>0.9495210000</t>
         </is>
       </c>
       <c r="M74" s="7" t="n"/>
@@ -4019,7 +4019,7 @@
       </c>
       <c r="L75" s="8" t="inlineStr">
         <is>
-          <t>1.4709390000</t>
+          <t>1.6567660000</t>
         </is>
       </c>
       <c r="M75" s="7" t="n"/>
@@ -4066,7 +4066,7 @@
       </c>
       <c r="L76" s="8" t="inlineStr">
         <is>
-          <t>1.3506390000</t>
+          <t>4.4983170000</t>
         </is>
       </c>
       <c r="M76" s="7" t="n"/>
@@ -4156,7 +4156,7 @@
       </c>
       <c r="L78" s="8" t="inlineStr">
         <is>
-          <t>65.7484890000</t>
+          <t>4.0395960000</t>
         </is>
       </c>
       <c r="M78" s="7" t="n"/>
@@ -4203,7 +4203,7 @@
       </c>
       <c r="L79" s="8" t="inlineStr">
         <is>
-          <t>1.1548690000</t>
+          <t>1.2007830000</t>
         </is>
       </c>
       <c r="M79" s="7" t="n"/>

</xml_diff>

<commit_message>
run parboil on CPU
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -1,12 +1,12 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -597,8 +597,10 @@
       <c r="J2" s="5" t="n">
         <v>18</v>
       </c>
-      <c r="K2" s="6" t="n">
-        <v>38.409191</v>
+      <c r="K2" s="6" t="inlineStr">
+        <is>
+          <t>6.4008760000</t>
+        </is>
       </c>
       <c r="L2" s="6" t="inlineStr">
         <is>
@@ -644,8 +646,10 @@
       <c r="J3" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="K3" s="6" t="n">
-        <v>553.3479</v>
+      <c r="K3" s="6" t="inlineStr">
+        <is>
+          <t>88.2381970000</t>
+        </is>
       </c>
       <c r="L3" s="6" t="inlineStr">
         <is>
@@ -691,7 +695,11 @@
       <c r="J4" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="K4" s="3" t="n"/>
+      <c r="K4" s="3" t="inlineStr">
+        <is>
+          <t>0.8518130000</t>
+        </is>
+      </c>
       <c r="L4" s="3" t="inlineStr">
         <is>
           <t>0.0021480000</t>
@@ -777,7 +785,11 @@
       <c r="J6" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="K6" s="3" t="n"/>
+      <c r="K6" s="3" t="inlineStr">
+        <is>
+          <t>1.4900190000</t>
+        </is>
+      </c>
       <c r="L6" s="3" t="inlineStr">
         <is>
           <t>0.0219260000</t>
@@ -820,7 +832,11 @@
       <c r="J7" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="K7" s="3" t="n"/>
+      <c r="K7" s="3" t="inlineStr">
+        <is>
+          <t>20.0798170000</t>
+        </is>
+      </c>
       <c r="L7" s="3" t="inlineStr">
         <is>
           <t>0.2361460000</t>

</xml_diff>

<commit_message>
fix rodinia pathfinder and run
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -470,7 +470,7 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O79"/>
+  <dimension ref="A1:O78"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -495,7 +495,7 @@
     <col width="13.57642857142857" bestFit="1" customWidth="1" style="13" min="15" max="15"/>
   </cols>
   <sheetData>
-    <row r="1" ht="18.75" customHeight="1">
+    <row r="1" ht="18" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
           <t>benchmark</t>
@@ -564,7 +564,7 @@
       <c r="N1" s="13" t="n"/>
       <c r="O1" s="13" t="n"/>
     </row>
-    <row r="2" ht="18.75" customHeight="1">
+    <row r="2" ht="18" customHeight="1">
       <c r="A2" s="1" t="inlineStr">
         <is>
           <t>parboil_cutcp</t>
@@ -613,7 +613,7 @@
       <c r="N2" s="13" t="n"/>
       <c r="O2" s="13" t="n"/>
     </row>
-    <row r="3" ht="18.75" customHeight="1">
+    <row r="3" ht="18" customHeight="1">
       <c r="A3" s="1" t="inlineStr">
         <is>
           <t>parboil_lbm</t>
@@ -662,7 +662,7 @@
       <c r="N3" s="13" t="n"/>
       <c r="O3" s="13" t="n"/>
     </row>
-    <row r="4" ht="18.75" customHeight="1">
+    <row r="4" ht="18" customHeight="1">
       <c r="A4" s="1" t="inlineStr">
         <is>
           <t>parboil_mri-q</t>
@@ -709,184 +709,188 @@
       <c r="N4" s="13" t="n"/>
       <c r="O4" s="13" t="n"/>
     </row>
-    <row r="5" ht="18.75" customHeight="1">
+    <row r="5" ht="18" customHeight="1">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>parboil_sgemm</t>
+          <t>parboil_stencil</t>
         </is>
       </c>
       <c r="B5" s="5" t="n">
         <v>0</v>
       </c>
       <c r="C5" s="5" t="n">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="D5" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="E5" s="5" t="n">
+        <v>6</v>
+      </c>
+      <c r="F5" s="5" t="n">
+        <v>10</v>
+      </c>
+      <c r="G5" s="5" t="n">
         <v>9</v>
       </c>
-      <c r="E5" s="5" t="n">
-        <v>8</v>
-      </c>
-      <c r="F5" s="5" t="n">
-        <v>6</v>
-      </c>
-      <c r="G5" s="5" t="n">
-        <v>6</v>
-      </c>
       <c r="H5" s="5" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="I5" s="5" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="J5" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="K5" s="3" t="n"/>
+      <c r="K5" s="3" t="inlineStr">
+        <is>
+          <t>1.4900190000</t>
+        </is>
+      </c>
       <c r="L5" s="3" t="inlineStr">
         <is>
-          <t>0.0002380000</t>
+          <t>0.0219260000</t>
         </is>
       </c>
       <c r="M5" s="2" t="n"/>
       <c r="N5" s="13" t="n"/>
       <c r="O5" s="13" t="n"/>
     </row>
-    <row r="6" ht="18.75" customHeight="1">
+    <row r="6" ht="18" customHeight="1">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>parboil_stencil</t>
+          <t>parboil_tpacf</t>
         </is>
       </c>
       <c r="B6" s="5" t="n">
         <v>0</v>
       </c>
       <c r="C6" s="5" t="n">
+        <v>66</v>
+      </c>
+      <c r="D6" s="5" t="n">
+        <v>54</v>
+      </c>
+      <c r="E6" s="5" t="n">
+        <v>14</v>
+      </c>
+      <c r="F6" s="5" t="n">
         <v>36</v>
       </c>
-      <c r="D6" s="5" t="n">
-        <v>3</v>
-      </c>
-      <c r="E6" s="5" t="n">
-        <v>6</v>
-      </c>
-      <c r="F6" s="5" t="n">
-        <v>10</v>
-      </c>
       <c r="G6" s="5" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="H6" s="5" t="n">
-        <v>16</v>
+        <v>77</v>
       </c>
       <c r="I6" s="5" t="n">
-        <v>4</v>
+        <v>53</v>
       </c>
       <c r="J6" s="5" t="n">
         <v>0</v>
       </c>
       <c r="K6" s="3" t="inlineStr">
         <is>
-          <t>1.4900190000</t>
+          <t>20.0798170000</t>
         </is>
       </c>
       <c r="L6" s="3" t="inlineStr">
         <is>
-          <t>0.0219260000</t>
+          <t>0.2361460000</t>
         </is>
       </c>
       <c r="M6" s="2" t="n"/>
       <c r="N6" s="13" t="n"/>
       <c r="O6" s="13" t="n"/>
     </row>
-    <row r="7" ht="18.75" customHeight="1">
+    <row r="7" ht="19.5" customHeight="1">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>parboil_tpacf</t>
-        </is>
-      </c>
-      <c r="B7" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="C7" s="5" t="n">
-        <v>66</v>
-      </c>
-      <c r="D7" s="5" t="n">
-        <v>54</v>
-      </c>
-      <c r="E7" s="5" t="n">
-        <v>14</v>
-      </c>
-      <c r="F7" s="5" t="n">
-        <v>36</v>
-      </c>
-      <c r="G7" s="5" t="n">
-        <v>7</v>
-      </c>
-      <c r="H7" s="5" t="n">
-        <v>77</v>
-      </c>
-      <c r="I7" s="5" t="n">
-        <v>53</v>
-      </c>
-      <c r="J7" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="K7" s="3" t="inlineStr">
-        <is>
-          <t>20.0798170000</t>
-        </is>
-      </c>
-      <c r="L7" s="3" t="inlineStr">
-        <is>
-          <t>0.2361460000</t>
-        </is>
-      </c>
-      <c r="M7" s="2" t="n"/>
+          <t>polybench_correlation</t>
+        </is>
+      </c>
+      <c r="B7" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="C7" s="7" t="n">
+        <v>81</v>
+      </c>
+      <c r="D7" s="7" t="n">
+        <v>40</v>
+      </c>
+      <c r="E7" s="7" t="n">
+        <v>15</v>
+      </c>
+      <c r="F7" s="7" t="n">
+        <v>17</v>
+      </c>
+      <c r="G7" s="7" t="n">
+        <v>19</v>
+      </c>
+      <c r="H7" s="7" t="n">
+        <v>59</v>
+      </c>
+      <c r="I7" s="7" t="n">
+        <v>32</v>
+      </c>
+      <c r="J7" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="K7" s="8" t="inlineStr">
+        <is>
+          <t>27.3023400000</t>
+        </is>
+      </c>
+      <c r="L7" s="8" t="inlineStr">
+        <is>
+          <t>1.3712850000</t>
+        </is>
+      </c>
+      <c r="M7" s="7" t="n"/>
       <c r="N7" s="13" t="n"/>
       <c r="O7" s="13" t="n"/>
     </row>
     <row r="8" ht="19.5" customHeight="1">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>polybench_correlation</t>
+          <t>polybench_covariance</t>
         </is>
       </c>
       <c r="B8" s="7" t="n">
         <v>0</v>
       </c>
       <c r="C8" s="7" t="n">
-        <v>81</v>
+        <v>53</v>
       </c>
       <c r="D8" s="7" t="n">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="E8" s="7" t="n">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="F8" s="7" t="n">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="G8" s="7" t="n">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="H8" s="7" t="n">
-        <v>59</v>
+        <v>36</v>
       </c>
       <c r="I8" s="7" t="n">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="J8" s="7" t="n">
         <v>0</v>
       </c>
       <c r="K8" s="8" t="inlineStr">
         <is>
-          <t>27.3023400000</t>
+          <t>26.8907790000</t>
         </is>
       </c>
       <c r="L8" s="8" t="inlineStr">
         <is>
-          <t>1.3712850000</t>
+          <t>1.3791970000</t>
         </is>
       </c>
       <c r="M8" s="7" t="n"/>
@@ -896,44 +900,44 @@
     <row r="9" ht="19.5" customHeight="1">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>polybench_covariance</t>
+          <t>polybench_2mm</t>
         </is>
       </c>
       <c r="B9" s="7" t="n">
         <v>0</v>
       </c>
       <c r="C9" s="7" t="n">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="D9" s="7" t="n">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="E9" s="7" t="n">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="F9" s="7" t="n">
         <v>12</v>
       </c>
       <c r="G9" s="7" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="H9" s="7" t="n">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I9" s="7" t="n">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="J9" s="7" t="n">
         <v>0</v>
       </c>
       <c r="K9" s="8" t="inlineStr">
         <is>
-          <t>26.8907790000</t>
+          <t>6.6711840000</t>
         </is>
       </c>
       <c r="L9" s="8" t="inlineStr">
         <is>
-          <t>1.3791970000</t>
+          <t>0.0046380000</t>
         </is>
       </c>
       <c r="M9" s="7" t="n"/>
@@ -943,44 +947,44 @@
     <row r="10" ht="19.5" customHeight="1">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>polybench_2mm</t>
+          <t>polybench_3mm</t>
         </is>
       </c>
       <c r="B10" s="7" t="n">
         <v>0</v>
       </c>
       <c r="C10" s="7" t="n">
-        <v>56</v>
+        <v>77</v>
       </c>
       <c r="D10" s="7" t="n">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="E10" s="7" t="n">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="F10" s="7" t="n">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="G10" s="7" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H10" s="7" t="n">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="I10" s="7" t="n">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="J10" s="7" t="n">
         <v>0</v>
       </c>
       <c r="K10" s="8" t="inlineStr">
         <is>
-          <t>6.6711840000</t>
+          <t>0.7054390000</t>
         </is>
       </c>
       <c r="L10" s="8" t="inlineStr">
         <is>
-          <t>0.0046380000</t>
+          <t>0.0011230000</t>
         </is>
       </c>
       <c r="M10" s="7" t="n"/>
@@ -990,44 +994,44 @@
     <row r="11" ht="19.5" customHeight="1">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>polybench_3mm</t>
+          <t>polybench_atax</t>
         </is>
       </c>
       <c r="B11" s="7" t="n">
         <v>0</v>
       </c>
       <c r="C11" s="7" t="n">
-        <v>77</v>
+        <v>36</v>
       </c>
       <c r="D11" s="7" t="n">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="E11" s="7" t="n">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="F11" s="7" t="n">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="G11" s="7" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="H11" s="7" t="n">
-        <v>51</v>
+        <v>34</v>
       </c>
       <c r="I11" s="7" t="n">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="J11" s="7" t="n">
         <v>0</v>
       </c>
       <c r="K11" s="8" t="inlineStr">
         <is>
-          <t>0.7054390000</t>
+          <t>0.0240260000</t>
         </is>
       </c>
       <c r="L11" s="8" t="inlineStr">
         <is>
-          <t>0.0011230000</t>
+          <t>0.0017900000</t>
         </is>
       </c>
       <c r="M11" s="7" t="n"/>
@@ -1037,7 +1041,7 @@
     <row r="12" ht="19.5" customHeight="1">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>polybench_atax</t>
+          <t>polybench_bicg</t>
         </is>
       </c>
       <c r="B12" s="7" t="n">
@@ -1062,19 +1066,19 @@
         <v>34</v>
       </c>
       <c r="I12" s="7" t="n">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="J12" s="7" t="n">
         <v>0</v>
       </c>
       <c r="K12" s="8" t="inlineStr">
         <is>
-          <t>0.0240260000</t>
+          <t>0.0462610000</t>
         </is>
       </c>
       <c r="L12" s="8" t="inlineStr">
         <is>
-          <t>0.0017900000</t>
+          <t>0.0020450000</t>
         </is>
       </c>
       <c r="M12" s="7" t="n"/>
@@ -1084,44 +1088,44 @@
     <row r="13" ht="19.5" customHeight="1">
       <c r="A13" s="1" t="inlineStr">
         <is>
-          <t>polybench_bicg</t>
+          <t>polybench_doitgen</t>
         </is>
       </c>
       <c r="B13" s="7" t="n">
         <v>0</v>
       </c>
       <c r="C13" s="7" t="n">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D13" s="7" t="n">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="E13" s="7" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F13" s="7" t="n">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="G13" s="7" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="H13" s="7" t="n">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="I13" s="7" t="n">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="J13" s="7" t="n">
         <v>0</v>
       </c>
       <c r="K13" s="8" t="inlineStr">
         <is>
-          <t>0.0462610000</t>
+          <t>0.3109120000</t>
         </is>
       </c>
       <c r="L13" s="8" t="inlineStr">
         <is>
-          <t>0.0020450000</t>
+          <t>0.0048460000</t>
         </is>
       </c>
       <c r="M13" s="7" t="n"/>
@@ -1131,44 +1135,44 @@
     <row r="14" ht="19.5" customHeight="1">
       <c r="A14" s="1" t="inlineStr">
         <is>
-          <t>polybench_doitgen</t>
+          <t>polybench_gemm</t>
         </is>
       </c>
       <c r="B14" s="7" t="n">
         <v>0</v>
       </c>
       <c r="C14" s="7" t="n">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D14" s="7" t="n">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E14" s="7" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F14" s="7" t="n">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="G14" s="7" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="H14" s="7" t="n">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I14" s="7" t="n">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="J14" s="7" t="n">
         <v>0</v>
       </c>
       <c r="K14" s="8" t="inlineStr">
         <is>
-          <t>0.3109120000</t>
+          <t>0.2416870000</t>
         </is>
       </c>
       <c r="L14" s="8" t="inlineStr">
         <is>
-          <t>0.0048460000</t>
+          <t>0.0003690000</t>
         </is>
       </c>
       <c r="M14" s="7" t="n"/>
@@ -1178,44 +1182,44 @@
     <row r="15" ht="19.5" customHeight="1">
       <c r="A15" s="1" t="inlineStr">
         <is>
-          <t>polybench_gemm</t>
+          <t>polybench_gemver</t>
         </is>
       </c>
       <c r="B15" s="7" t="n">
         <v>0</v>
       </c>
       <c r="C15" s="7" t="n">
-        <v>31</v>
+        <v>51</v>
       </c>
       <c r="D15" s="7" t="n">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="E15" s="7" t="n">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="F15" s="7" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="G15" s="7" t="n">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="H15" s="7" t="n">
-        <v>18</v>
+        <v>50</v>
       </c>
       <c r="I15" s="7" t="n">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="J15" s="7" t="n">
         <v>0</v>
       </c>
       <c r="K15" s="8" t="inlineStr">
         <is>
-          <t>0.2416870000</t>
+          <t>0.1402210000</t>
         </is>
       </c>
       <c r="L15" s="8" t="inlineStr">
         <is>
-          <t>0.0003690000</t>
+          <t>0.0022660000</t>
         </is>
       </c>
       <c r="M15" s="7" t="n"/>
@@ -1225,44 +1229,44 @@
     <row r="16" ht="19.5" customHeight="1">
       <c r="A16" s="1" t="inlineStr">
         <is>
-          <t>polybench_gemver</t>
+          <t>polybench_gesummv</t>
         </is>
       </c>
       <c r="B16" s="7" t="n">
         <v>0</v>
       </c>
       <c r="C16" s="7" t="n">
-        <v>51</v>
+        <v>13</v>
       </c>
       <c r="D16" s="7" t="n">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="E16" s="7" t="n">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="F16" s="7" t="n">
+        <v>3</v>
+      </c>
+      <c r="G16" s="7" t="n">
+        <v>5</v>
+      </c>
+      <c r="H16" s="7" t="n">
+        <v>18</v>
+      </c>
+      <c r="I16" s="7" t="n">
         <v>9</v>
       </c>
-      <c r="G16" s="7" t="n">
-        <v>17</v>
-      </c>
-      <c r="H16" s="7" t="n">
-        <v>50</v>
-      </c>
-      <c r="I16" s="7" t="n">
-        <v>21</v>
-      </c>
       <c r="J16" s="7" t="n">
         <v>0</v>
       </c>
       <c r="K16" s="8" t="inlineStr">
         <is>
-          <t>0.1402210000</t>
+          <t>0.0459630000</t>
         </is>
       </c>
       <c r="L16" s="8" t="inlineStr">
         <is>
-          <t>0.0022660000</t>
+          <t>0.0016130000</t>
         </is>
       </c>
       <c r="M16" s="7" t="n"/>
@@ -1272,44 +1276,44 @@
     <row r="17" ht="19.5" customHeight="1">
       <c r="A17" s="1" t="inlineStr">
         <is>
-          <t>polybench_gesummv</t>
+          <t>polybench_mvt</t>
         </is>
       </c>
       <c r="B17" s="7" t="n">
         <v>0</v>
       </c>
       <c r="C17" s="7" t="n">
-        <v>13</v>
+        <v>36</v>
       </c>
       <c r="D17" s="7" t="n">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="E17" s="7" t="n">
+        <v>10</v>
+      </c>
+      <c r="F17" s="7" t="n">
         <v>6</v>
       </c>
-      <c r="F17" s="7" t="n">
-        <v>3</v>
-      </c>
       <c r="G17" s="7" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="H17" s="7" t="n">
-        <v>18</v>
+        <v>34</v>
       </c>
       <c r="I17" s="7" t="n">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="J17" s="7" t="n">
         <v>0</v>
       </c>
       <c r="K17" s="8" t="inlineStr">
         <is>
-          <t>0.0459630000</t>
+          <t>0.1371760000</t>
         </is>
       </c>
       <c r="L17" s="8" t="inlineStr">
         <is>
-          <t>0.0016130000</t>
+          <t>0.0017880000</t>
         </is>
       </c>
       <c r="M17" s="7" t="n"/>
@@ -1319,20 +1323,20 @@
     <row r="18" ht="19.5" customHeight="1">
       <c r="A18" s="1" t="inlineStr">
         <is>
-          <t>polybench_mvt</t>
+          <t>polybench_syr2k</t>
         </is>
       </c>
       <c r="B18" s="7" t="n">
         <v>0</v>
       </c>
       <c r="C18" s="7" t="n">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="D18" s="7" t="n">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="E18" s="7" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="F18" s="7" t="n">
         <v>6</v>
@@ -1341,22 +1345,22 @@
         <v>7</v>
       </c>
       <c r="H18" s="7" t="n">
-        <v>34</v>
+        <v>12</v>
       </c>
       <c r="I18" s="7" t="n">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="J18" s="7" t="n">
         <v>0</v>
       </c>
       <c r="K18" s="8" t="inlineStr">
         <is>
-          <t>0.1371760000</t>
+          <t>2.5838750000</t>
         </is>
       </c>
       <c r="L18" s="8" t="inlineStr">
         <is>
-          <t>0.0017880000</t>
+          <t>0.0168660000</t>
         </is>
       </c>
       <c r="M18" s="7" t="n"/>
@@ -1366,44 +1370,44 @@
     <row r="19" ht="19.5" customHeight="1">
       <c r="A19" s="1" t="inlineStr">
         <is>
-          <t>polybench_syr2k</t>
+          <t>polybench_syrk</t>
         </is>
       </c>
       <c r="B19" s="7" t="n">
         <v>0</v>
       </c>
       <c r="C19" s="7" t="n">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="D19" s="7" t="n">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="E19" s="7" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F19" s="7" t="n">
         <v>6</v>
       </c>
       <c r="G19" s="7" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H19" s="7" t="n">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="I19" s="7" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="J19" s="7" t="n">
         <v>0</v>
       </c>
       <c r="K19" s="8" t="inlineStr">
         <is>
-          <t>2.5838750000</t>
+          <t>1.2780200000</t>
         </is>
       </c>
       <c r="L19" s="8" t="inlineStr">
         <is>
-          <t>0.0168660000</t>
+          <t>0.0086670000</t>
         </is>
       </c>
       <c r="M19" s="7" t="n"/>
@@ -1413,44 +1417,44 @@
     <row r="20" ht="19.5" customHeight="1">
       <c r="A20" s="1" t="inlineStr">
         <is>
-          <t>polybench_syrk</t>
+          <t>polybench_gramschmidt</t>
         </is>
       </c>
       <c r="B20" s="7" t="n">
         <v>0</v>
       </c>
       <c r="C20" s="7" t="n">
+        <v>86</v>
+      </c>
+      <c r="D20" s="7" t="n">
+        <v>19</v>
+      </c>
+      <c r="E20" s="7" t="n">
+        <v>18</v>
+      </c>
+      <c r="F20" s="7" t="n">
+        <v>18</v>
+      </c>
+      <c r="G20" s="7" t="n">
+        <v>18</v>
+      </c>
+      <c r="H20" s="7" t="n">
+        <v>58</v>
+      </c>
+      <c r="I20" s="7" t="n">
         <v>29</v>
       </c>
-      <c r="D20" s="7" t="n">
-        <v>9</v>
-      </c>
-      <c r="E20" s="7" t="n">
-        <v>7</v>
-      </c>
-      <c r="F20" s="7" t="n">
-        <v>6</v>
-      </c>
-      <c r="G20" s="7" t="n">
-        <v>8</v>
-      </c>
-      <c r="H20" s="7" t="n">
-        <v>18</v>
-      </c>
-      <c r="I20" s="7" t="n">
-        <v>10</v>
-      </c>
       <c r="J20" s="7" t="n">
         <v>0</v>
       </c>
       <c r="K20" s="8" t="inlineStr">
         <is>
-          <t>1.2780200000</t>
+          <t>77.0461650000</t>
         </is>
       </c>
       <c r="L20" s="8" t="inlineStr">
         <is>
-          <t>0.0086670000</t>
+          <t>2.1602340000</t>
         </is>
       </c>
       <c r="M20" s="7" t="n"/>
@@ -1460,44 +1464,44 @@
     <row r="21" ht="19.5" customHeight="1">
       <c r="A21" s="1" t="inlineStr">
         <is>
-          <t>polybench_gramschmidt</t>
+          <t>polybench_lu</t>
         </is>
       </c>
       <c r="B21" s="7" t="n">
         <v>0</v>
       </c>
       <c r="C21" s="7" t="n">
-        <v>86</v>
+        <v>21</v>
       </c>
       <c r="D21" s="7" t="n">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="E21" s="7" t="n">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="F21" s="7" t="n">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="G21" s="7" t="n">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="H21" s="7" t="n">
-        <v>58</v>
+        <v>12</v>
       </c>
       <c r="I21" s="7" t="n">
-        <v>29</v>
+        <v>8</v>
       </c>
       <c r="J21" s="7" t="n">
         <v>0</v>
       </c>
       <c r="K21" s="8" t="inlineStr">
         <is>
-          <t>77.0461650000</t>
+          <t>0.5386620000</t>
         </is>
       </c>
       <c r="L21" s="8" t="inlineStr">
         <is>
-          <t>2.1602340000</t>
+          <t>0.0552200000</t>
         </is>
       </c>
       <c r="M21" s="7" t="n"/>
@@ -1507,44 +1511,44 @@
     <row r="22" ht="19.5" customHeight="1">
       <c r="A22" s="1" t="inlineStr">
         <is>
-          <t>polybench_lu</t>
+          <t>polybench_adi</t>
         </is>
       </c>
       <c r="B22" s="7" t="n">
         <v>0</v>
       </c>
       <c r="C22" s="7" t="n">
-        <v>21</v>
+        <v>75</v>
       </c>
       <c r="D22" s="7" t="n">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="E22" s="7" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="F22" s="7" t="n">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="G22" s="7" t="n">
-        <v>4</v>
+        <v>27</v>
       </c>
       <c r="H22" s="7" t="n">
-        <v>12</v>
+        <v>74</v>
       </c>
       <c r="I22" s="7" t="n">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="J22" s="7" t="n">
         <v>0</v>
       </c>
       <c r="K22" s="8" t="inlineStr">
         <is>
-          <t>0.5386620000</t>
+          <t>0.0095040000</t>
         </is>
       </c>
       <c r="L22" s="8" t="inlineStr">
         <is>
-          <t>0.0552200000</t>
+          <t>0.0179850000</t>
         </is>
       </c>
       <c r="M22" s="7" t="n"/>
@@ -1554,44 +1558,44 @@
     <row r="23" ht="19.5" customHeight="1">
       <c r="A23" s="1" t="inlineStr">
         <is>
-          <t>polybench_adi</t>
+          <t>polybench_convolution-2d</t>
         </is>
       </c>
       <c r="B23" s="7" t="n">
         <v>0</v>
       </c>
       <c r="C23" s="7" t="n">
-        <v>75</v>
+        <v>34</v>
       </c>
       <c r="D23" s="7" t="n">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="E23" s="7" t="n">
+        <v>12</v>
+      </c>
+      <c r="F23" s="7" t="n">
+        <v>11</v>
+      </c>
+      <c r="G23" s="7" t="n">
         <v>10</v>
       </c>
-      <c r="F23" s="7" t="n">
-        <v>24</v>
-      </c>
-      <c r="G23" s="7" t="n">
-        <v>27</v>
-      </c>
       <c r="H23" s="7" t="n">
-        <v>74</v>
+        <v>20</v>
       </c>
       <c r="I23" s="7" t="n">
-        <v>24</v>
+        <v>5</v>
       </c>
       <c r="J23" s="7" t="n">
         <v>0</v>
       </c>
       <c r="K23" s="8" t="inlineStr">
         <is>
-          <t>0.0095040000</t>
+          <t>0.0316410000</t>
         </is>
       </c>
       <c r="L23" s="8" t="inlineStr">
         <is>
-          <t>0.0179850000</t>
+          <t>0.0003940000</t>
         </is>
       </c>
       <c r="M23" s="7" t="n"/>
@@ -1601,44 +1605,44 @@
     <row r="24" ht="19.5" customHeight="1">
       <c r="A24" s="1" t="inlineStr">
         <is>
-          <t>polybench_convolution-2d</t>
+          <t>polybench_convolution-3d</t>
         </is>
       </c>
       <c r="B24" s="7" t="n">
         <v>0</v>
       </c>
       <c r="C24" s="7" t="n">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="D24" s="7" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E24" s="7" t="n">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="F24" s="7" t="n">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="G24" s="7" t="n">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="H24" s="7" t="n">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="I24" s="7" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="J24" s="7" t="n">
         <v>0</v>
       </c>
       <c r="K24" s="8" t="inlineStr">
         <is>
-          <t>0.0316410000</t>
+          <t>0.0436070000</t>
         </is>
       </c>
       <c r="L24" s="8" t="inlineStr">
         <is>
-          <t>0.0003940000</t>
+          <t>0.0008070000</t>
         </is>
       </c>
       <c r="M24" s="7" t="n"/>
@@ -1648,44 +1652,44 @@
     <row r="25" ht="19.5" customHeight="1">
       <c r="A25" s="1" t="inlineStr">
         <is>
-          <t>polybench_convolution-3d</t>
+          <t>polybench_fdtd-2d</t>
         </is>
       </c>
       <c r="B25" s="7" t="n">
         <v>0</v>
       </c>
       <c r="C25" s="7" t="n">
-        <v>60</v>
+        <v>38</v>
       </c>
       <c r="D25" s="7" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E25" s="7" t="n">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="F25" s="7" t="n">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="G25" s="7" t="n">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="H25" s="7" t="n">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="I25" s="7" t="n">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="J25" s="7" t="n">
         <v>0</v>
       </c>
       <c r="K25" s="8" t="inlineStr">
         <is>
-          <t>0.0436070000</t>
+          <t>4.5973770000</t>
         </is>
       </c>
       <c r="L25" s="8" t="inlineStr">
         <is>
-          <t>0.0008070000</t>
+          <t>0.1137690000</t>
         </is>
       </c>
       <c r="M25" s="7" t="n"/>
@@ -1695,44 +1699,44 @@
     <row r="26" ht="19.5" customHeight="1">
       <c r="A26" s="1" t="inlineStr">
         <is>
-          <t>polybench_fdtd-2d</t>
+          <t>polybench_jacobi-1d-imper</t>
         </is>
       </c>
       <c r="B26" s="7" t="n">
         <v>0</v>
       </c>
       <c r="C26" s="7" t="n">
-        <v>38</v>
+        <v>14</v>
       </c>
       <c r="D26" s="7" t="n">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E26" s="7" t="n">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="F26" s="7" t="n">
-        <v>26</v>
+        <v>4</v>
       </c>
       <c r="G26" s="7" t="n">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="H26" s="7" t="n">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="I26" s="7" t="n">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="J26" s="7" t="n">
         <v>0</v>
       </c>
       <c r="K26" s="8" t="inlineStr">
         <is>
-          <t>4.5973770000</t>
+          <t>0.0289850000</t>
         </is>
       </c>
       <c r="L26" s="8" t="inlineStr">
         <is>
-          <t>0.1137690000</t>
+          <t>0.1370770000</t>
         </is>
       </c>
       <c r="M26" s="7" t="n"/>
@@ -1742,44 +1746,44 @@
     <row r="27" ht="19.5" customHeight="1">
       <c r="A27" s="1" t="inlineStr">
         <is>
-          <t>polybench_jacobi-1d-imper</t>
+          <t>polybench_jacobi-2d-imper</t>
         </is>
       </c>
       <c r="B27" s="7" t="n">
         <v>0</v>
       </c>
       <c r="C27" s="7" t="n">
-        <v>14</v>
+        <v>30</v>
       </c>
       <c r="D27" s="7" t="n">
+        <v>8</v>
+      </c>
+      <c r="E27" s="7" t="n">
+        <v>6</v>
+      </c>
+      <c r="F27" s="7" t="n">
         <v>12</v>
       </c>
-      <c r="E27" s="7" t="n">
-        <v>4</v>
-      </c>
-      <c r="F27" s="7" t="n">
-        <v>4</v>
-      </c>
       <c r="G27" s="7" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H27" s="7" t="n">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="I27" s="7" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="J27" s="7" t="n">
         <v>0</v>
       </c>
       <c r="K27" s="8" t="inlineStr">
         <is>
-          <t>0.0289850000</t>
+          <t>0.0123620000</t>
         </is>
       </c>
       <c r="L27" s="8" t="inlineStr">
         <is>
-          <t>0.1370770000</t>
+          <t>0.0007230000</t>
         </is>
       </c>
       <c r="M27" s="7" t="n"/>
@@ -1789,44 +1793,44 @@
     <row r="28" ht="19.5" customHeight="1">
       <c r="A28" s="1" t="inlineStr">
         <is>
-          <t>polybench_jacobi-2d-imper</t>
+          <t>amd_AtomicCounters</t>
         </is>
       </c>
       <c r="B28" s="7" t="n">
         <v>0</v>
       </c>
       <c r="C28" s="7" t="n">
-        <v>30</v>
+        <v>4</v>
       </c>
       <c r="D28" s="7" t="n">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="E28" s="7" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F28" s="7" t="n">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="G28" s="7" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H28" s="7" t="n">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="I28" s="7" t="n">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="J28" s="7" t="n">
         <v>0</v>
       </c>
       <c r="K28" s="8" t="inlineStr">
         <is>
-          <t>0.0123620000</t>
+          <t>0.0528379000</t>
         </is>
       </c>
       <c r="L28" s="8" t="inlineStr">
         <is>
-          <t>0.0007230000</t>
+          <t>0.0003475150</t>
         </is>
       </c>
       <c r="M28" s="7" t="n"/>
@@ -1836,44 +1840,44 @@
     <row r="29" ht="19.5" customHeight="1">
       <c r="A29" s="1" t="inlineStr">
         <is>
-          <t>amd_AtomicCounters</t>
+          <t>amd_BinarySearch</t>
         </is>
       </c>
       <c r="B29" s="7" t="n">
         <v>0</v>
       </c>
       <c r="C29" s="7" t="n">
-        <v>4</v>
+        <v>32</v>
       </c>
       <c r="D29" s="7" t="n">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="E29" s="7" t="n">
         <v>5</v>
       </c>
       <c r="F29" s="7" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="G29" s="7" t="n">
         <v>0</v>
       </c>
       <c r="H29" s="7" t="n">
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="I29" s="7" t="n">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="J29" s="7" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="K29" s="8" t="inlineStr">
         <is>
-          <t>0.0528379000</t>
+          <t>0.0140000000</t>
         </is>
       </c>
       <c r="L29" s="8" t="inlineStr">
         <is>
-          <t>0.0003475150</t>
+          <t>0.0060000000</t>
         </is>
       </c>
       <c r="M29" s="7" t="n"/>
@@ -1883,44 +1887,44 @@
     <row r="30" ht="19.5" customHeight="1">
       <c r="A30" s="1" t="inlineStr">
         <is>
-          <t>amd_BinarySearch</t>
+          <t>amd_BinomialOption</t>
         </is>
       </c>
       <c r="B30" s="7" t="n">
         <v>0</v>
       </c>
       <c r="C30" s="7" t="n">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="D30" s="7" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E30" s="7" t="n">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="F30" s="7" t="n">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="G30" s="7" t="n">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="H30" s="7" t="n">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="I30" s="7" t="n">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="J30" s="7" t="n">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="K30" s="8" t="inlineStr">
         <is>
-          <t>0.0140000000</t>
+          <t>0.5789000000</t>
         </is>
       </c>
       <c r="L30" s="8" t="inlineStr">
         <is>
-          <t>0.0060000000</t>
+          <t>0.5760600000</t>
         </is>
       </c>
       <c r="M30" s="7" t="n"/>
@@ -1930,44 +1934,44 @@
     <row r="31" ht="19.5" customHeight="1">
       <c r="A31" s="1" t="inlineStr">
         <is>
-          <t>amd_BinomialOption</t>
+          <t>amd_BitonicSort</t>
         </is>
       </c>
       <c r="B31" s="7" t="n">
         <v>0</v>
       </c>
       <c r="C31" s="7" t="n">
-        <v>38</v>
+        <v>11</v>
       </c>
       <c r="D31" s="7" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E31" s="7" t="n">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="F31" s="7" t="n">
         <v>3</v>
       </c>
       <c r="G31" s="7" t="n">
-        <v>34</v>
+        <v>0</v>
       </c>
       <c r="H31" s="7" t="n">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="I31" s="7" t="n">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="J31" s="7" t="n">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="K31" s="8" t="inlineStr">
         <is>
-          <t>0.5789000000</t>
+          <t>0.4280000000</t>
         </is>
       </c>
       <c r="L31" s="8" t="inlineStr">
         <is>
-          <t>0.5760600000</t>
+          <t>0.1030000000</t>
         </is>
       </c>
       <c r="M31" s="7" t="n"/>
@@ -1977,44 +1981,44 @@
     <row r="32" ht="19.5" customHeight="1">
       <c r="A32" s="1" t="inlineStr">
         <is>
-          <t>amd_BitonicSort</t>
+          <t>amd_BlackScholes</t>
         </is>
       </c>
       <c r="B32" s="7" t="n">
         <v>0</v>
       </c>
       <c r="C32" s="7" t="n">
-        <v>11</v>
+        <v>159</v>
       </c>
       <c r="D32" s="7" t="n">
+        <v>12</v>
+      </c>
+      <c r="E32" s="7" t="n">
+        <v>103</v>
+      </c>
+      <c r="F32" s="7" t="n">
+        <v>2</v>
+      </c>
+      <c r="G32" s="7" t="n">
+        <v>178</v>
+      </c>
+      <c r="H32" s="7" t="n">
         <v>14</v>
       </c>
-      <c r="E32" s="7" t="n">
-        <v>3</v>
-      </c>
-      <c r="F32" s="7" t="n">
-        <v>3</v>
-      </c>
-      <c r="G32" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="H32" s="7" t="n">
-        <v>6</v>
-      </c>
       <c r="I32" s="7" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="J32" s="7" t="n">
         <v>0</v>
       </c>
       <c r="K32" s="8" t="inlineStr">
         <is>
-          <t>0.4280000000</t>
+          <t>0.6647100000</t>
         </is>
       </c>
       <c r="L32" s="8" t="inlineStr">
         <is>
-          <t>0.1030000000</t>
+          <t>0.6865900000</t>
         </is>
       </c>
       <c r="M32" s="7" t="n"/>
@@ -2024,44 +2028,44 @@
     <row r="33" ht="19.5" customHeight="1">
       <c r="A33" s="1" t="inlineStr">
         <is>
-          <t>amd_BlackScholes</t>
+          <t>amd_BlackScholesDP</t>
         </is>
       </c>
       <c r="B33" s="7" t="n">
         <v>0</v>
       </c>
       <c r="C33" s="7" t="n">
-        <v>159</v>
+        <v>82</v>
       </c>
       <c r="D33" s="7" t="n">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="E33" s="7" t="n">
-        <v>103</v>
+        <v>71</v>
       </c>
       <c r="F33" s="7" t="n">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="G33" s="7" t="n">
-        <v>178</v>
+        <v>91</v>
       </c>
       <c r="H33" s="7" t="n">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="I33" s="7" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J33" s="7" t="n">
         <v>0</v>
       </c>
       <c r="K33" s="8" t="inlineStr">
         <is>
-          <t>0.6647100000</t>
+          <t>0.6452500000</t>
         </is>
       </c>
       <c r="L33" s="8" t="inlineStr">
         <is>
-          <t>0.6865900000</t>
+          <t>0.7585000000</t>
         </is>
       </c>
       <c r="M33" s="7" t="n"/>
@@ -2071,44 +2075,44 @@
     <row r="34" ht="19.5" customHeight="1">
       <c r="A34" s="1" t="inlineStr">
         <is>
-          <t>amd_BlackScholesDP</t>
+          <t>amd_BoxFilter</t>
         </is>
       </c>
       <c r="B34" s="7" t="n">
         <v>0</v>
       </c>
       <c r="C34" s="7" t="n">
-        <v>82</v>
+        <v>146</v>
       </c>
       <c r="D34" s="7" t="n">
-        <v>21</v>
+        <v>58</v>
       </c>
       <c r="E34" s="7" t="n">
-        <v>71</v>
+        <v>50</v>
       </c>
       <c r="F34" s="7" t="n">
-        <v>9</v>
+        <v>88</v>
       </c>
       <c r="G34" s="7" t="n">
-        <v>91</v>
+        <v>0</v>
       </c>
       <c r="H34" s="7" t="n">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="I34" s="7" t="n">
-        <v>4</v>
+        <v>54</v>
       </c>
       <c r="J34" s="7" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="K34" s="8" t="inlineStr">
         <is>
-          <t>0.6452500000</t>
+          <t>0.7257500000</t>
         </is>
       </c>
       <c r="L34" s="8" t="inlineStr">
         <is>
-          <t>0.7585000000</t>
+          <t>0.7711400000</t>
         </is>
       </c>
       <c r="M34" s="7" t="n"/>
@@ -2118,44 +2122,44 @@
     <row r="35" ht="19.5" customHeight="1">
       <c r="A35" s="1" t="inlineStr">
         <is>
-          <t>amd_BoxFilter</t>
+          <t>amd_BufferImageInterop</t>
         </is>
       </c>
       <c r="B35" s="7" t="n">
         <v>0</v>
       </c>
       <c r="C35" s="7" t="n">
-        <v>146</v>
+        <v>20</v>
       </c>
       <c r="D35" s="7" t="n">
-        <v>58</v>
+        <v>12</v>
       </c>
       <c r="E35" s="7" t="n">
-        <v>50</v>
+        <v>16</v>
       </c>
       <c r="F35" s="7" t="n">
-        <v>88</v>
+        <v>16</v>
       </c>
       <c r="G35" s="7" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="H35" s="7" t="n">
-        <v>60</v>
+        <v>7</v>
       </c>
       <c r="I35" s="7" t="n">
-        <v>54</v>
+        <v>3</v>
       </c>
       <c r="J35" s="7" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="K35" s="8" t="inlineStr">
         <is>
-          <t>0.7257500000</t>
+          <t>0.3880000000</t>
         </is>
       </c>
       <c r="L35" s="8" t="inlineStr">
         <is>
-          <t>0.7711400000</t>
+          <t>0.0110000000</t>
         </is>
       </c>
       <c r="M35" s="7" t="n"/>
@@ -2163,46 +2167,46 @@
       <c r="O35" s="13" t="n"/>
     </row>
     <row r="36" ht="19.5" customHeight="1">
-      <c r="A36" s="1" t="inlineStr">
-        <is>
-          <t>amd_BufferImageInterop</t>
+      <c r="A36" s="9" t="inlineStr">
+        <is>
+          <t>amd_DCT</t>
         </is>
       </c>
       <c r="B36" s="7" t="n">
         <v>0</v>
       </c>
       <c r="C36" s="7" t="n">
-        <v>20</v>
+        <v>73</v>
       </c>
       <c r="D36" s="7" t="n">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E36" s="7" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F36" s="7" t="n">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="G36" s="7" t="n">
         <v>7</v>
       </c>
       <c r="H36" s="7" t="n">
-        <v>7</v>
+        <v>28</v>
       </c>
       <c r="I36" s="7" t="n">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="J36" s="7" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="K36" s="8" t="inlineStr">
         <is>
-          <t>0.3880000000</t>
+          <t>0.6890500000</t>
         </is>
       </c>
       <c r="L36" s="8" t="inlineStr">
         <is>
-          <t>0.0110000000</t>
+          <t>0.5800300000</t>
         </is>
       </c>
       <c r="M36" s="7" t="n"/>
@@ -2210,46 +2214,46 @@
       <c r="O36" s="13" t="n"/>
     </row>
     <row r="37" ht="19.5" customHeight="1">
-      <c r="A37" s="9" t="inlineStr">
-        <is>
-          <t>amd_DCT</t>
+      <c r="A37" s="1" t="inlineStr">
+        <is>
+          <t>amd_DwtHaar1D</t>
         </is>
       </c>
       <c r="B37" s="7" t="n">
         <v>0</v>
       </c>
       <c r="C37" s="7" t="n">
-        <v>73</v>
+        <v>27</v>
       </c>
       <c r="D37" s="7" t="n">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="E37" s="7" t="n">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="F37" s="7" t="n">
-        <v>28</v>
+        <v>5</v>
       </c>
       <c r="G37" s="7" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H37" s="7" t="n">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="I37" s="7" t="n">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="J37" s="7" t="n">
         <v>0</v>
       </c>
       <c r="K37" s="8" t="inlineStr">
         <is>
-          <t>0.6890500000</t>
+          <t>0.6660800000</t>
         </is>
       </c>
       <c r="L37" s="8" t="inlineStr">
         <is>
-          <t>0.5800300000</t>
+          <t>0.6761200000</t>
         </is>
       </c>
       <c r="M37" s="7" t="n"/>
@@ -2259,44 +2263,44 @@
     <row r="38" ht="19.5" customHeight="1">
       <c r="A38" s="1" t="inlineStr">
         <is>
-          <t>amd_DwtHaar1D</t>
+          <t>amd_FastWalshTransform</t>
         </is>
       </c>
       <c r="B38" s="7" t="n">
         <v>0</v>
       </c>
       <c r="C38" s="7" t="n">
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="D38" s="7" t="n">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="E38" s="7" t="n">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="F38" s="7" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G38" s="7" t="n">
+        <v>2</v>
+      </c>
+      <c r="H38" s="7" t="n">
         <v>6</v>
       </c>
-      <c r="H38" s="7" t="n">
-        <v>18</v>
-      </c>
       <c r="I38" s="7" t="n">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="J38" s="7" t="n">
         <v>0</v>
       </c>
       <c r="K38" s="8" t="inlineStr">
         <is>
-          <t>0.6660800000</t>
+          <t>0.6112400000</t>
         </is>
       </c>
       <c r="L38" s="8" t="inlineStr">
         <is>
-          <t>0.6761200000</t>
+          <t>0.6751200000</t>
         </is>
       </c>
       <c r="M38" s="7" t="n"/>
@@ -2306,7 +2310,7 @@
     <row r="39" ht="19.5" customHeight="1">
       <c r="A39" s="1" t="inlineStr">
         <is>
-          <t>amd_FastWalshTransform</t>
+          <t>amd_FloydWarshall</t>
         </is>
       </c>
       <c r="B39" s="7" t="n">
@@ -2316,34 +2320,34 @@
         <v>9</v>
       </c>
       <c r="D39" s="7" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E39" s="7" t="n">
+        <v>4</v>
+      </c>
+      <c r="F39" s="7" t="n">
+        <v>5</v>
+      </c>
+      <c r="G39" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H39" s="7" t="n">
+        <v>9</v>
+      </c>
+      <c r="I39" s="7" t="n">
         <v>3</v>
       </c>
-      <c r="F39" s="7" t="n">
-        <v>3</v>
-      </c>
-      <c r="G39" s="7" t="n">
-        <v>2</v>
-      </c>
-      <c r="H39" s="7" t="n">
-        <v>6</v>
-      </c>
-      <c r="I39" s="7" t="n">
-        <v>1</v>
-      </c>
       <c r="J39" s="7" t="n">
         <v>0</v>
       </c>
       <c r="K39" s="8" t="inlineStr">
         <is>
-          <t>0.6112400000</t>
+          <t>0.6583600000</t>
         </is>
       </c>
       <c r="L39" s="8" t="inlineStr">
         <is>
-          <t>0.6751200000</t>
+          <t>0.6565700000</t>
         </is>
       </c>
       <c r="M39" s="7" t="n"/>
@@ -2353,44 +2357,44 @@
     <row r="40" ht="19.5" customHeight="1">
       <c r="A40" s="1" t="inlineStr">
         <is>
-          <t>amd_FloydWarshall</t>
+          <t>amd_ImageOverlap</t>
         </is>
       </c>
       <c r="B40" s="7" t="n">
         <v>0</v>
       </c>
       <c r="C40" s="7" t="n">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D40" s="7" t="n">
         <v>4</v>
       </c>
       <c r="E40" s="7" t="n">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="F40" s="7" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G40" s="7" t="n">
         <v>0</v>
       </c>
       <c r="H40" s="7" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="I40" s="7" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J40" s="7" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K40" s="8" t="inlineStr">
         <is>
-          <t>0.6583600000</t>
+          <t>0.6252900000</t>
         </is>
       </c>
       <c r="L40" s="8" t="inlineStr">
         <is>
-          <t>0.6565700000</t>
+          <t>0.5911300000</t>
         </is>
       </c>
       <c r="M40" s="7" t="n"/>
@@ -2400,44 +2404,44 @@
     <row r="41" ht="19.5" customHeight="1">
       <c r="A41" s="1" t="inlineStr">
         <is>
-          <t>amd_ImageOverlap</t>
+          <t>amd_LUDecomposition</t>
         </is>
       </c>
       <c r="B41" s="7" t="n">
         <v>0</v>
       </c>
       <c r="C41" s="7" t="n">
-        <v>6</v>
+        <v>46</v>
       </c>
       <c r="D41" s="7" t="n">
-        <v>4</v>
+        <v>34</v>
       </c>
       <c r="E41" s="7" t="n">
+        <v>17</v>
+      </c>
+      <c r="F41" s="7" t="n">
+        <v>17</v>
+      </c>
+      <c r="G41" s="7" t="n">
         <v>10</v>
       </c>
-      <c r="F41" s="7" t="n">
-        <v>3</v>
-      </c>
-      <c r="G41" s="7" t="n">
-        <v>0</v>
-      </c>
       <c r="H41" s="7" t="n">
-        <v>0</v>
+        <v>59</v>
       </c>
       <c r="I41" s="7" t="n">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="J41" s="7" t="n">
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="K41" s="8" t="inlineStr">
         <is>
-          <t>0.6252900000</t>
+          <t>0.6474900000</t>
         </is>
       </c>
       <c r="L41" s="8" t="inlineStr">
         <is>
-          <t>0.5911300000</t>
+          <t>0.6041900000</t>
         </is>
       </c>
       <c r="M41" s="7" t="n"/>
@@ -2447,44 +2451,44 @@
     <row r="42" ht="19.5" customHeight="1">
       <c r="A42" s="1" t="inlineStr">
         <is>
-          <t>amd_LUDecomposition</t>
+          <t>amd_MatrixMulImage</t>
         </is>
       </c>
       <c r="B42" s="7" t="n">
         <v>0</v>
       </c>
       <c r="C42" s="7" t="n">
-        <v>46</v>
+        <v>271</v>
       </c>
       <c r="D42" s="7" t="n">
-        <v>34</v>
+        <v>101</v>
       </c>
       <c r="E42" s="7" t="n">
-        <v>17</v>
+        <v>326</v>
       </c>
       <c r="F42" s="7" t="n">
-        <v>17</v>
+        <v>70</v>
       </c>
       <c r="G42" s="7" t="n">
-        <v>10</v>
+        <v>250</v>
       </c>
       <c r="H42" s="7" t="n">
-        <v>59</v>
+        <v>0</v>
       </c>
       <c r="I42" s="7" t="n">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="J42" s="7" t="n">
-        <v>30</v>
+        <v>332</v>
       </c>
       <c r="K42" s="8" t="inlineStr">
         <is>
-          <t>0.6474900000</t>
+          <t>0.6949400000</t>
         </is>
       </c>
       <c r="L42" s="8" t="inlineStr">
         <is>
-          <t>0.6041900000</t>
+          <t>0.5711200000</t>
         </is>
       </c>
       <c r="M42" s="7" t="n"/>
@@ -2494,44 +2498,44 @@
     <row r="43" ht="19.5" customHeight="1">
       <c r="A43" s="1" t="inlineStr">
         <is>
-          <t>amd_MatrixMulImage</t>
+          <t>amd_MatrixMultiplication</t>
         </is>
       </c>
       <c r="B43" s="7" t="n">
         <v>0</v>
       </c>
       <c r="C43" s="7" t="n">
-        <v>271</v>
+        <v>240</v>
       </c>
       <c r="D43" s="7" t="n">
-        <v>101</v>
+        <v>54</v>
       </c>
       <c r="E43" s="7" t="n">
-        <v>326</v>
+        <v>110</v>
       </c>
       <c r="F43" s="7" t="n">
-        <v>70</v>
+        <v>25</v>
       </c>
       <c r="G43" s="7" t="n">
-        <v>250</v>
+        <v>161</v>
       </c>
       <c r="H43" s="7" t="n">
-        <v>0</v>
+        <v>64</v>
       </c>
       <c r="I43" s="7" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J43" s="7" t="n">
-        <v>332</v>
+        <v>128</v>
       </c>
       <c r="K43" s="8" t="inlineStr">
         <is>
-          <t>0.6949400000</t>
+          <t>0.7830000000</t>
         </is>
       </c>
       <c r="L43" s="8" t="inlineStr">
         <is>
-          <t>0.5711200000</t>
+          <t>0.5740000000</t>
         </is>
       </c>
       <c r="M43" s="7" t="n"/>
@@ -2541,44 +2545,44 @@
     <row r="44" ht="19.5" customHeight="1">
       <c r="A44" s="1" t="inlineStr">
         <is>
-          <t>amd_MatrixMultiplication</t>
+          <t>amd_MatrixTranspose</t>
         </is>
       </c>
       <c r="B44" s="7" t="n">
         <v>0</v>
       </c>
       <c r="C44" s="7" t="n">
-        <v>240</v>
+        <v>37</v>
       </c>
       <c r="D44" s="7" t="n">
-        <v>54</v>
+        <v>29</v>
       </c>
       <c r="E44" s="7" t="n">
-        <v>110</v>
+        <v>11</v>
       </c>
       <c r="F44" s="7" t="n">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G44" s="7" t="n">
-        <v>161</v>
+        <v>0</v>
       </c>
       <c r="H44" s="7" t="n">
-        <v>64</v>
+        <v>32</v>
       </c>
       <c r="I44" s="7" t="n">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="J44" s="7" t="n">
-        <v>128</v>
+        <v>12</v>
       </c>
       <c r="K44" s="8" t="inlineStr">
         <is>
-          <t>0.7830000000</t>
+          <t>0.6440800000</t>
         </is>
       </c>
       <c r="L44" s="8" t="inlineStr">
         <is>
-          <t>0.5740000000</t>
+          <t>0.5640800000</t>
         </is>
       </c>
       <c r="M44" s="7" t="n"/>
@@ -2588,44 +2592,44 @@
     <row r="45" ht="19.5" customHeight="1">
       <c r="A45" s="1" t="inlineStr">
         <is>
-          <t>amd_MatrixTranspose</t>
+          <t>amd_MonteCarloAsian</t>
         </is>
       </c>
       <c r="B45" s="7" t="n">
         <v>0</v>
       </c>
       <c r="C45" s="7" t="n">
+        <v>153</v>
+      </c>
+      <c r="D45" s="7" t="n">
+        <v>320</v>
+      </c>
+      <c r="E45" s="7" t="n">
+        <v>70</v>
+      </c>
+      <c r="F45" s="7" t="n">
         <v>37</v>
       </c>
-      <c r="D45" s="7" t="n">
-        <v>29</v>
-      </c>
-      <c r="E45" s="7" t="n">
-        <v>11</v>
-      </c>
-      <c r="F45" s="7" t="n">
-        <v>23</v>
-      </c>
       <c r="G45" s="7" t="n">
-        <v>0</v>
+        <v>96</v>
       </c>
       <c r="H45" s="7" t="n">
-        <v>32</v>
+        <v>120</v>
       </c>
       <c r="I45" s="7" t="n">
-        <v>1</v>
+        <v>46</v>
       </c>
       <c r="J45" s="7" t="n">
-        <v>12</v>
+        <v>115</v>
       </c>
       <c r="K45" s="8" t="inlineStr">
         <is>
-          <t>0.6440800000</t>
+          <t>23.4670000000</t>
         </is>
       </c>
       <c r="L45" s="8" t="inlineStr">
         <is>
-          <t>0.5640800000</t>
+          <t>0.3470000000</t>
         </is>
       </c>
       <c r="M45" s="7" t="n"/>
@@ -2635,44 +2639,44 @@
     <row r="46" ht="19.5" customHeight="1">
       <c r="A46" s="1" t="inlineStr">
         <is>
-          <t>amd_MonteCarloAsian</t>
+          <t>amd_MonteCarloAsianDP</t>
         </is>
       </c>
       <c r="B46" s="7" t="n">
         <v>0</v>
       </c>
       <c r="C46" s="7" t="n">
-        <v>153</v>
+        <v>56</v>
       </c>
       <c r="D46" s="7" t="n">
-        <v>320</v>
+        <v>134</v>
       </c>
       <c r="E46" s="7" t="n">
-        <v>70</v>
+        <v>31</v>
       </c>
       <c r="F46" s="7" t="n">
-        <v>37</v>
+        <v>8</v>
       </c>
       <c r="G46" s="7" t="n">
-        <v>96</v>
+        <v>51</v>
       </c>
       <c r="H46" s="7" t="n">
-        <v>120</v>
+        <v>75</v>
       </c>
       <c r="I46" s="7" t="n">
-        <v>46</v>
+        <v>18</v>
       </c>
       <c r="J46" s="7" t="n">
-        <v>115</v>
+        <v>84</v>
       </c>
       <c r="K46" s="8" t="inlineStr">
         <is>
-          <t>23.4670000000</t>
+          <t>1.2809300000</t>
         </is>
       </c>
       <c r="L46" s="8" t="inlineStr">
         <is>
-          <t>0.3470000000</t>
+          <t>0.7104400000</t>
         </is>
       </c>
       <c r="M46" s="7" t="n"/>
@@ -2682,44 +2686,44 @@
     <row r="47" ht="19.5" customHeight="1">
       <c r="A47" s="1" t="inlineStr">
         <is>
-          <t>amd_MonteCarloAsianDP</t>
+          <t>amd_PrefixSum</t>
         </is>
       </c>
       <c r="B47" s="7" t="n">
         <v>0</v>
       </c>
       <c r="C47" s="7" t="n">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="D47" s="7" t="n">
-        <v>134</v>
+        <v>33</v>
       </c>
       <c r="E47" s="7" t="n">
+        <v>13</v>
+      </c>
+      <c r="F47" s="7" t="n">
+        <v>29</v>
+      </c>
+      <c r="G47" s="7" t="n">
+        <v>3</v>
+      </c>
+      <c r="H47" s="7" t="n">
         <v>31</v>
       </c>
-      <c r="F47" s="7" t="n">
-        <v>8</v>
-      </c>
-      <c r="G47" s="7" t="n">
-        <v>51</v>
-      </c>
-      <c r="H47" s="7" t="n">
-        <v>75</v>
-      </c>
       <c r="I47" s="7" t="n">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="J47" s="7" t="n">
-        <v>84</v>
+        <v>0</v>
       </c>
       <c r="K47" s="8" t="inlineStr">
         <is>
-          <t>1.2809300000</t>
+          <t>0.0140000000</t>
         </is>
       </c>
       <c r="L47" s="8" t="inlineStr">
         <is>
-          <t>0.7104400000</t>
+          <t>0.0020000000</t>
         </is>
       </c>
       <c r="M47" s="7" t="n"/>
@@ -2729,44 +2733,44 @@
     <row r="48" ht="19.5" customHeight="1">
       <c r="A48" s="1" t="inlineStr">
         <is>
-          <t>amd_PrefixSum</t>
+          <t>amd_QuasiRandomSequence</t>
         </is>
       </c>
       <c r="B48" s="7" t="n">
         <v>0</v>
       </c>
       <c r="C48" s="7" t="n">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="D48" s="7" t="n">
-        <v>33</v>
+        <v>95</v>
       </c>
       <c r="E48" s="7" t="n">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="F48" s="7" t="n">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="G48" s="7" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H48" s="7" t="n">
-        <v>31</v>
+        <v>55</v>
       </c>
       <c r="I48" s="7" t="n">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="J48" s="7" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="K48" s="8" t="inlineStr">
         <is>
-          <t>0.0140000000</t>
+          <t>0.0050000000</t>
         </is>
       </c>
       <c r="L48" s="8" t="inlineStr">
         <is>
-          <t>0.0020000000</t>
+          <t>0.0010000000</t>
         </is>
       </c>
       <c r="M48" s="7" t="n"/>
@@ -2776,44 +2780,44 @@
     <row r="49" ht="19.5" customHeight="1">
       <c r="A49" s="1" t="inlineStr">
         <is>
-          <t>amd_QuasiRandomSequence</t>
+          <t>amd_RadixSort</t>
         </is>
       </c>
       <c r="B49" s="7" t="n">
         <v>0</v>
       </c>
       <c r="C49" s="7" t="n">
-        <v>40</v>
+        <v>83</v>
       </c>
       <c r="D49" s="7" t="n">
-        <v>95</v>
+        <v>72</v>
       </c>
       <c r="E49" s="7" t="n">
-        <v>18</v>
+        <v>38</v>
       </c>
       <c r="F49" s="7" t="n">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="G49" s="7" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H49" s="7" t="n">
-        <v>55</v>
+        <v>92</v>
       </c>
       <c r="I49" s="7" t="n">
-        <v>8</v>
+        <v>33</v>
       </c>
       <c r="J49" s="7" t="n">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="K49" s="8" t="inlineStr">
         <is>
-          <t>0.0050000000</t>
+          <t>0.1110000000</t>
         </is>
       </c>
       <c r="L49" s="8" t="inlineStr">
         <is>
-          <t>0.0010000000</t>
+          <t>0.0610000000</t>
         </is>
       </c>
       <c r="M49" s="7" t="n"/>
@@ -2823,44 +2827,44 @@
     <row r="50" ht="19.5" customHeight="1">
       <c r="A50" s="1" t="inlineStr">
         <is>
-          <t>amd_RadixSort</t>
+          <t>amd_RecursiveGaussian</t>
         </is>
       </c>
       <c r="B50" s="7" t="n">
         <v>0</v>
       </c>
       <c r="C50" s="7" t="n">
-        <v>83</v>
+        <v>31</v>
       </c>
       <c r="D50" s="7" t="n">
-        <v>72</v>
+        <v>17</v>
       </c>
       <c r="E50" s="7" t="n">
-        <v>38</v>
+        <v>16</v>
       </c>
       <c r="F50" s="7" t="n">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="G50" s="7" t="n">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="H50" s="7" t="n">
-        <v>92</v>
+        <v>16</v>
       </c>
       <c r="I50" s="7" t="n">
-        <v>33</v>
+        <v>10</v>
       </c>
       <c r="J50" s="7" t="n">
-        <v>0</v>
+        <v>56</v>
       </c>
       <c r="K50" s="8" t="inlineStr">
         <is>
-          <t>0.1110000000</t>
+          <t>0.5719000000</t>
         </is>
       </c>
       <c r="L50" s="8" t="inlineStr">
         <is>
-          <t>0.0610000000</t>
+          <t>0.6849700000</t>
         </is>
       </c>
       <c r="M50" s="7" t="n"/>
@@ -2870,44 +2874,44 @@
     <row r="51" ht="19.5" customHeight="1">
       <c r="A51" s="1" t="inlineStr">
         <is>
-          <t>amd_RecursiveGaussian</t>
+          <t>amd_Reduction</t>
         </is>
       </c>
       <c r="B51" s="7" t="n">
         <v>0</v>
       </c>
       <c r="C51" s="7" t="n">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="D51" s="7" t="n">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="E51" s="7" t="n">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="F51" s="7" t="n">
-        <v>37</v>
+        <v>6</v>
       </c>
       <c r="G51" s="7" t="n">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="H51" s="7" t="n">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="I51" s="7" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="J51" s="7" t="n">
-        <v>56</v>
+        <v>0</v>
       </c>
       <c r="K51" s="8" t="inlineStr">
         <is>
-          <t>0.5719000000</t>
+          <t>0.6080700000</t>
         </is>
       </c>
       <c r="L51" s="8" t="inlineStr">
         <is>
-          <t>0.6849700000</t>
+          <t>0.6690400000</t>
         </is>
       </c>
       <c r="M51" s="7" t="n"/>
@@ -2917,44 +2921,44 @@
     <row r="52" ht="19.5" customHeight="1">
       <c r="A52" s="1" t="inlineStr">
         <is>
-          <t>amd_Reduction</t>
+          <t>amd_ScanLargeArrays</t>
         </is>
       </c>
       <c r="B52" s="7" t="n">
         <v>0</v>
       </c>
       <c r="C52" s="7" t="n">
-        <v>13</v>
+        <v>31</v>
       </c>
       <c r="D52" s="7" t="n">
-        <v>13</v>
+        <v>36</v>
       </c>
       <c r="E52" s="7" t="n">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="F52" s="7" t="n">
-        <v>6</v>
+        <v>38</v>
       </c>
       <c r="G52" s="7" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="H52" s="7" t="n">
-        <v>13</v>
+        <v>67</v>
       </c>
       <c r="I52" s="7" t="n">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="J52" s="7" t="n">
         <v>0</v>
       </c>
       <c r="K52" s="8" t="inlineStr">
         <is>
-          <t>0.6080700000</t>
+          <t>0.0130000000</t>
         </is>
       </c>
       <c r="L52" s="8" t="inlineStr">
         <is>
-          <t>0.6690400000</t>
+          <t>0.0030000000</t>
         </is>
       </c>
       <c r="M52" s="7" t="n"/>
@@ -2964,44 +2968,44 @@
     <row r="53" ht="19.5" customHeight="1">
       <c r="A53" s="1" t="inlineStr">
         <is>
-          <t>amd_ScanLargeArrays</t>
+          <t>amd_SimpleConvolution</t>
         </is>
       </c>
       <c r="B53" s="7" t="n">
         <v>0</v>
       </c>
       <c r="C53" s="7" t="n">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D53" s="7" t="n">
-        <v>36</v>
+        <v>7</v>
       </c>
       <c r="E53" s="7" t="n">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="F53" s="7" t="n">
-        <v>38</v>
+        <v>5</v>
       </c>
       <c r="G53" s="7" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="H53" s="7" t="n">
-        <v>67</v>
+        <v>6</v>
       </c>
       <c r="I53" s="7" t="n">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="J53" s="7" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="K53" s="8" t="inlineStr">
         <is>
-          <t>0.0130000000</t>
+          <t>0.5607500000</t>
         </is>
       </c>
       <c r="L53" s="8" t="inlineStr">
         <is>
-          <t>0.0030000000</t>
+          <t>0.7050300000</t>
         </is>
       </c>
       <c r="M53" s="7" t="n"/>
@@ -3011,44 +3015,44 @@
     <row r="54" ht="19.5" customHeight="1">
       <c r="A54" s="1" t="inlineStr">
         <is>
-          <t>amd_SimpleConvolution</t>
+          <t>amd_SimpleImage</t>
         </is>
       </c>
       <c r="B54" s="7" t="n">
         <v>0</v>
       </c>
       <c r="C54" s="7" t="n">
-        <v>32</v>
+        <v>10</v>
       </c>
       <c r="D54" s="7" t="n">
+        <v>9</v>
+      </c>
+      <c r="E54" s="7" t="n">
+        <v>17</v>
+      </c>
+      <c r="F54" s="7" t="n">
         <v>7</v>
       </c>
-      <c r="E54" s="7" t="n">
-        <v>6</v>
-      </c>
-      <c r="F54" s="7" t="n">
-        <v>5</v>
-      </c>
       <c r="G54" s="7" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H54" s="7" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="I54" s="7" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="J54" s="7" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="K54" s="8" t="inlineStr">
         <is>
-          <t>0.5607500000</t>
+          <t>0.5937400000</t>
         </is>
       </c>
       <c r="L54" s="8" t="inlineStr">
         <is>
-          <t>0.7050300000</t>
+          <t>0.6913200000</t>
         </is>
       </c>
       <c r="M54" s="7" t="n"/>
@@ -3058,44 +3062,44 @@
     <row r="55" ht="19.5" customHeight="1">
       <c r="A55" s="1" t="inlineStr">
         <is>
-          <t>amd_SimpleImage</t>
+          <t>amd_SobelFilter</t>
         </is>
       </c>
       <c r="B55" s="7" t="n">
         <v>0</v>
       </c>
       <c r="C55" s="7" t="n">
-        <v>10</v>
+        <v>34</v>
       </c>
       <c r="D55" s="7" t="n">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E55" s="7" t="n">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="F55" s="7" t="n">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="G55" s="7" t="n">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="H55" s="7" t="n">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="I55" s="7" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="J55" s="7" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="K55" s="8" t="inlineStr">
         <is>
-          <t>0.5937400000</t>
+          <t>0.5751100000</t>
         </is>
       </c>
       <c r="L55" s="8" t="inlineStr">
         <is>
-          <t>0.6913200000</t>
+          <t>0.6692100000</t>
         </is>
       </c>
       <c r="M55" s="7" t="n"/>
@@ -3105,44 +3109,44 @@
     <row r="56" ht="19.5" customHeight="1">
       <c r="A56" s="1" t="inlineStr">
         <is>
-          <t>amd_SobelFilter</t>
+          <t>amd_StringSearch</t>
         </is>
       </c>
       <c r="B56" s="7" t="n">
         <v>0</v>
       </c>
       <c r="C56" s="7" t="n">
-        <v>34</v>
+        <v>87</v>
       </c>
       <c r="D56" s="7" t="n">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="E56" s="7" t="n">
         <v>20</v>
       </c>
       <c r="F56" s="7" t="n">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="G56" s="7" t="n">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="H56" s="7" t="n">
-        <v>18</v>
+        <v>51</v>
       </c>
       <c r="I56" s="7" t="n">
-        <v>5</v>
+        <v>43</v>
       </c>
       <c r="J56" s="7" t="n">
         <v>0</v>
       </c>
       <c r="K56" s="8" t="inlineStr">
         <is>
-          <t>0.5751100000</t>
+          <t>0.0380000000</t>
         </is>
       </c>
       <c r="L56" s="8" t="inlineStr">
         <is>
-          <t>0.6692100000</t>
+          <t>0.0240000000</t>
         </is>
       </c>
       <c r="M56" s="7" t="n"/>
@@ -3152,44 +3156,44 @@
     <row r="57" ht="19.5" customHeight="1">
       <c r="A57" s="1" t="inlineStr">
         <is>
-          <t>amd_StringSearch</t>
+          <t>amd_TransferOverlap</t>
         </is>
       </c>
       <c r="B57" s="7" t="n">
         <v>0</v>
       </c>
       <c r="C57" s="7" t="n">
-        <v>87</v>
+        <v>49</v>
       </c>
       <c r="D57" s="7" t="n">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E57" s="7" t="n">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="F57" s="7" t="n">
-        <v>30</v>
+        <v>4</v>
       </c>
       <c r="G57" s="7" t="n">
         <v>0</v>
       </c>
       <c r="H57" s="7" t="n">
-        <v>51</v>
+        <v>25</v>
       </c>
       <c r="I57" s="7" t="n">
-        <v>43</v>
+        <v>24</v>
       </c>
       <c r="J57" s="7" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="K57" s="8" t="inlineStr">
         <is>
-          <t>0.0380000000</t>
+          <t>4.3045000000</t>
         </is>
       </c>
       <c r="L57" s="8" t="inlineStr">
         <is>
-          <t>0.0240000000</t>
+          <t>0.5590070000</t>
         </is>
       </c>
       <c r="M57" s="7" t="n"/>
@@ -3199,44 +3203,44 @@
     <row r="58" ht="19.5" customHeight="1">
       <c r="A58" s="1" t="inlineStr">
         <is>
-          <t>amd_TransferOverlap</t>
+          <t>amd_URNG</t>
         </is>
       </c>
       <c r="B58" s="7" t="n">
         <v>0</v>
       </c>
       <c r="C58" s="7" t="n">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="D58" s="7" t="n">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="E58" s="7" t="n">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="F58" s="7" t="n">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="G58" s="7" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="H58" s="7" t="n">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="I58" s="7" t="n">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="J58" s="7" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="K58" s="8" t="inlineStr">
         <is>
-          <t>4.3045000000</t>
+          <t>0.6114800000</t>
         </is>
       </c>
       <c r="L58" s="8" t="inlineStr">
         <is>
-          <t>0.5590070000</t>
+          <t>0.6673300000</t>
         </is>
       </c>
       <c r="M58" s="7" t="n"/>
@@ -3246,44 +3250,44 @@
     <row r="59" ht="19.5" customHeight="1">
       <c r="A59" s="1" t="inlineStr">
         <is>
-          <t>amd_URNG</t>
+          <t>rodinia_b+tree</t>
         </is>
       </c>
       <c r="B59" s="7" t="n">
         <v>0</v>
       </c>
       <c r="C59" s="7" t="n">
-        <v>52</v>
+        <v>13</v>
       </c>
       <c r="D59" s="7" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E59" s="7" t="n">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="F59" s="7" t="n">
+        <v>3</v>
+      </c>
+      <c r="G59" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H59" s="7" t="n">
+        <v>25</v>
+      </c>
+      <c r="I59" s="7" t="n">
         <v>12</v>
       </c>
-      <c r="G59" s="7" t="n">
-        <v>9</v>
-      </c>
-      <c r="H59" s="7" t="n">
-        <v>16</v>
-      </c>
-      <c r="I59" s="7" t="n">
-        <v>10</v>
-      </c>
       <c r="J59" s="7" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="K59" s="8" t="inlineStr">
         <is>
-          <t>0.6114800000</t>
+          <t>0.0823160000</t>
         </is>
       </c>
       <c r="L59" s="8" t="inlineStr">
         <is>
-          <t>0.6673300000</t>
+          <t>1.1325580000</t>
         </is>
       </c>
       <c r="M59" s="7" t="n"/>
@@ -3293,44 +3297,44 @@
     <row r="60" ht="19.5" customHeight="1">
       <c r="A60" s="1" t="inlineStr">
         <is>
-          <t>rodinia_b+tree</t>
+          <t>rodinia_backprop</t>
         </is>
       </c>
       <c r="B60" s="7" t="n">
         <v>0</v>
       </c>
       <c r="C60" s="7" t="n">
-        <v>13</v>
+        <v>56</v>
       </c>
       <c r="D60" s="7" t="n">
+        <v>38</v>
+      </c>
+      <c r="E60" s="7" t="n">
+        <v>23</v>
+      </c>
+      <c r="F60" s="7" t="n">
+        <v>23</v>
+      </c>
+      <c r="G60" s="7" t="n">
+        <v>19</v>
+      </c>
+      <c r="H60" s="7" t="n">
+        <v>58</v>
+      </c>
+      <c r="I60" s="7" t="n">
         <v>18</v>
       </c>
-      <c r="E60" s="7" t="n">
-        <v>7</v>
-      </c>
-      <c r="F60" s="7" t="n">
-        <v>3</v>
-      </c>
-      <c r="G60" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="H60" s="7" t="n">
-        <v>25</v>
-      </c>
-      <c r="I60" s="7" t="n">
-        <v>12</v>
-      </c>
       <c r="J60" s="7" t="n">
         <v>0</v>
       </c>
       <c r="K60" s="8" t="inlineStr">
         <is>
-          <t>0.0823160000</t>
+          <t>0.6391930000</t>
         </is>
       </c>
       <c r="L60" s="8" t="inlineStr">
         <is>
-          <t>1.1325580000</t>
+          <t>1.2671750000</t>
         </is>
       </c>
       <c r="M60" s="7" t="n"/>
@@ -3338,46 +3342,46 @@
       <c r="O60" s="13" t="n"/>
     </row>
     <row r="61" ht="19.5" customHeight="1">
-      <c r="A61" s="1" t="inlineStr">
-        <is>
-          <t>rodinia_backprop</t>
+      <c r="A61" s="9" t="inlineStr">
+        <is>
+          <t>rodinia_bfs</t>
         </is>
       </c>
       <c r="B61" s="7" t="n">
         <v>0</v>
       </c>
       <c r="C61" s="7" t="n">
-        <v>56</v>
+        <v>13</v>
       </c>
       <c r="D61" s="7" t="n">
-        <v>38</v>
+        <v>13</v>
       </c>
       <c r="E61" s="7" t="n">
-        <v>23</v>
+        <v>4</v>
       </c>
       <c r="F61" s="7" t="n">
-        <v>23</v>
+        <v>5</v>
       </c>
       <c r="G61" s="7" t="n">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="H61" s="7" t="n">
-        <v>58</v>
+        <v>27</v>
       </c>
       <c r="I61" s="7" t="n">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="J61" s="7" t="n">
         <v>0</v>
       </c>
       <c r="K61" s="8" t="inlineStr">
         <is>
-          <t>0.6391930000</t>
+          <t>0.1200500000</t>
         </is>
       </c>
       <c r="L61" s="8" t="inlineStr">
         <is>
-          <t>1.2671750000</t>
+          <t>0.8565370000</t>
         </is>
       </c>
       <c r="M61" s="7" t="n"/>
@@ -3385,46 +3389,46 @@
       <c r="O61" s="13" t="n"/>
     </row>
     <row r="62" ht="19.5" customHeight="1">
-      <c r="A62" s="9" t="inlineStr">
-        <is>
-          <t>rodinia_bfs</t>
+      <c r="A62" s="1" t="inlineStr">
+        <is>
+          <t>rodinia_cfd</t>
         </is>
       </c>
       <c r="B62" s="7" t="n">
         <v>0</v>
       </c>
       <c r="C62" s="7" t="n">
-        <v>13</v>
+        <v>511</v>
       </c>
       <c r="D62" s="7" t="n">
-        <v>13</v>
+        <v>46</v>
       </c>
       <c r="E62" s="7" t="n">
-        <v>4</v>
+        <v>224</v>
       </c>
       <c r="F62" s="7" t="n">
-        <v>5</v>
+        <v>51</v>
       </c>
       <c r="G62" s="7" t="n">
-        <v>0</v>
+        <v>466</v>
       </c>
       <c r="H62" s="7" t="n">
-        <v>27</v>
+        <v>234</v>
       </c>
       <c r="I62" s="7" t="n">
-        <v>12</v>
+        <v>36</v>
       </c>
       <c r="J62" s="7" t="n">
         <v>0</v>
       </c>
       <c r="K62" s="8" t="inlineStr">
         <is>
-          <t>0.1200500000</t>
+          <t>8.6193270000</t>
         </is>
       </c>
       <c r="L62" s="8" t="inlineStr">
         <is>
-          <t>0.8565370000</t>
+          <t>1.9598740000</t>
         </is>
       </c>
       <c r="M62" s="7" t="n"/>
@@ -3434,44 +3438,44 @@
     <row r="63" ht="19.5" customHeight="1">
       <c r="A63" s="1" t="inlineStr">
         <is>
-          <t>rodinia_cfd</t>
+          <t>rodinia_dwt2d</t>
         </is>
       </c>
       <c r="B63" s="7" t="n">
         <v>0</v>
       </c>
       <c r="C63" s="7" t="n">
-        <v>511</v>
+        <v>453</v>
       </c>
       <c r="D63" s="7" t="n">
-        <v>46</v>
+        <v>268</v>
       </c>
       <c r="E63" s="7" t="n">
-        <v>224</v>
+        <v>50</v>
       </c>
       <c r="F63" s="7" t="n">
-        <v>51</v>
+        <v>94</v>
       </c>
       <c r="G63" s="7" t="n">
-        <v>466</v>
+        <v>0</v>
       </c>
       <c r="H63" s="7" t="n">
-        <v>234</v>
+        <v>428</v>
       </c>
       <c r="I63" s="7" t="n">
-        <v>36</v>
+        <v>149</v>
       </c>
       <c r="J63" s="7" t="n">
         <v>0</v>
       </c>
       <c r="K63" s="8" t="inlineStr">
         <is>
-          <t>8.6193270000</t>
+          <t>0.1033040000</t>
         </is>
       </c>
       <c r="L63" s="8" t="inlineStr">
         <is>
-          <t>1.9598740000</t>
+          <t>0.8027820000</t>
         </is>
       </c>
       <c r="M63" s="7" t="n"/>
@@ -3481,44 +3485,44 @@
     <row r="64" ht="19.5" customHeight="1">
       <c r="A64" s="1" t="inlineStr">
         <is>
-          <t>rodinia_dwt2d</t>
+          <t>rodinia_gaussian</t>
         </is>
       </c>
       <c r="B64" s="7" t="n">
         <v>0</v>
       </c>
       <c r="C64" s="7" t="n">
-        <v>453</v>
+        <v>25</v>
       </c>
       <c r="D64" s="7" t="n">
-        <v>268</v>
+        <v>8</v>
       </c>
       <c r="E64" s="7" t="n">
-        <v>50</v>
+        <v>7</v>
       </c>
       <c r="F64" s="7" t="n">
-        <v>94</v>
+        <v>11</v>
       </c>
       <c r="G64" s="7" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="H64" s="7" t="n">
-        <v>428</v>
+        <v>23</v>
       </c>
       <c r="I64" s="7" t="n">
-        <v>149</v>
+        <v>8</v>
       </c>
       <c r="J64" s="7" t="n">
         <v>0</v>
       </c>
       <c r="K64" s="8" t="inlineStr">
         <is>
-          <t>0.1033040000</t>
+          <t>4.0266510000</t>
         </is>
       </c>
       <c r="L64" s="8" t="inlineStr">
         <is>
-          <t>0.8027820000</t>
+          <t>1.1964120000</t>
         </is>
       </c>
       <c r="M64" s="7" t="n"/>
@@ -3528,44 +3532,44 @@
     <row r="65" ht="19.5" customHeight="1">
       <c r="A65" s="1" t="inlineStr">
         <is>
-          <t>rodinia_gaussian</t>
+          <t>rodinia_heartwall</t>
         </is>
       </c>
       <c r="B65" s="7" t="n">
         <v>0</v>
       </c>
       <c r="C65" s="7" t="n">
-        <v>25</v>
+        <v>678</v>
       </c>
       <c r="D65" s="7" t="n">
-        <v>8</v>
+        <v>261</v>
       </c>
       <c r="E65" s="7" t="n">
-        <v>7</v>
+        <v>50</v>
       </c>
       <c r="F65" s="7" t="n">
-        <v>11</v>
+        <v>163</v>
       </c>
       <c r="G65" s="7" t="n">
-        <v>6</v>
+        <v>97</v>
       </c>
       <c r="H65" s="7" t="n">
-        <v>23</v>
+        <v>679</v>
       </c>
       <c r="I65" s="7" t="n">
-        <v>8</v>
+        <v>225</v>
       </c>
       <c r="J65" s="7" t="n">
         <v>0</v>
       </c>
       <c r="K65" s="8" t="inlineStr">
         <is>
-          <t>4.0266510000</t>
+          <t>12.3171850000</t>
         </is>
       </c>
       <c r="L65" s="8" t="inlineStr">
         <is>
-          <t>1.1964120000</t>
+          <t>1.2765400000</t>
         </is>
       </c>
       <c r="M65" s="7" t="n"/>
@@ -3575,44 +3579,44 @@
     <row r="66" ht="19.5" customHeight="1">
       <c r="A66" s="1" t="inlineStr">
         <is>
-          <t>rodinia_heartwall</t>
+          <t>rodinia_hotspot</t>
         </is>
       </c>
       <c r="B66" s="7" t="n">
         <v>0</v>
       </c>
       <c r="C66" s="7" t="n">
-        <v>678</v>
+        <v>65</v>
       </c>
       <c r="D66" s="7" t="n">
-        <v>261</v>
+        <v>29</v>
       </c>
       <c r="E66" s="7" t="n">
-        <v>50</v>
+        <v>16</v>
       </c>
       <c r="F66" s="7" t="n">
-        <v>163</v>
+        <v>18</v>
       </c>
       <c r="G66" s="7" t="n">
-        <v>97</v>
+        <v>14</v>
       </c>
       <c r="H66" s="7" t="n">
-        <v>679</v>
+        <v>28</v>
       </c>
       <c r="I66" s="7" t="n">
-        <v>225</v>
+        <v>16</v>
       </c>
       <c r="J66" s="7" t="n">
         <v>0</v>
       </c>
       <c r="K66" s="8" t="inlineStr">
         <is>
-          <t>12.3171850000</t>
+          <t>32.7613950000</t>
         </is>
       </c>
       <c r="L66" s="8" t="inlineStr">
         <is>
-          <t>1.2765400000</t>
+          <t>1.3033110000</t>
         </is>
       </c>
       <c r="M66" s="7" t="n"/>
@@ -3622,44 +3626,44 @@
     <row r="67" ht="19.5" customHeight="1">
       <c r="A67" s="1" t="inlineStr">
         <is>
-          <t>rodinia_hotspot</t>
+          <t>rodinia_hotspot3D</t>
         </is>
       </c>
       <c r="B67" s="7" t="n">
         <v>0</v>
       </c>
       <c r="C67" s="7" t="n">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="D67" s="7" t="n">
-        <v>29</v>
+        <v>7</v>
       </c>
       <c r="E67" s="7" t="n">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="F67" s="7" t="n">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="G67" s="7" t="n">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="H67" s="7" t="n">
-        <v>28</v>
+        <v>42</v>
       </c>
       <c r="I67" s="7" t="n">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="J67" s="7" t="n">
         <v>0</v>
       </c>
       <c r="K67" s="8" t="inlineStr">
         <is>
-          <t>32.7613950000</t>
+          <t>0.9711030000</t>
         </is>
       </c>
       <c r="L67" s="8" t="inlineStr">
         <is>
-          <t>1.3033110000</t>
+          <t>0.2607990000</t>
         </is>
       </c>
       <c r="M67" s="7" t="n"/>
@@ -3669,44 +3673,44 @@
     <row r="68" ht="19.5" customHeight="1">
       <c r="A68" s="1" t="inlineStr">
         <is>
-          <t>rodinia_hotspot3D</t>
+          <t>rodinia_hybridsort</t>
         </is>
       </c>
       <c r="B68" s="7" t="n">
         <v>0</v>
       </c>
       <c r="C68" s="7" t="n">
+        <v>106</v>
+      </c>
+      <c r="D68" s="7" t="n">
+        <v>84</v>
+      </c>
+      <c r="E68" s="7" t="n">
+        <v>30</v>
+      </c>
+      <c r="F68" s="7" t="n">
+        <v>48</v>
+      </c>
+      <c r="G68" s="7" t="n">
         <v>67</v>
       </c>
-      <c r="D68" s="7" t="n">
-        <v>7</v>
-      </c>
-      <c r="E68" s="7" t="n">
-        <v>28</v>
-      </c>
-      <c r="F68" s="7" t="n">
-        <v>24</v>
-      </c>
-      <c r="G68" s="7" t="n">
-        <v>28</v>
-      </c>
       <c r="H68" s="7" t="n">
-        <v>42</v>
+        <v>110</v>
       </c>
       <c r="I68" s="7" t="n">
-        <v>6</v>
+        <v>55</v>
       </c>
       <c r="J68" s="7" t="n">
-        <v>0</v>
+        <v>58</v>
       </c>
       <c r="K68" s="8" t="inlineStr">
         <is>
-          <t>0.9711030000</t>
+          <t>0.2438150000</t>
         </is>
       </c>
       <c r="L68" s="8" t="inlineStr">
         <is>
-          <t>0.2607990000</t>
+          <t>0.3520820000</t>
         </is>
       </c>
       <c r="M68" s="7" t="n"/>
@@ -3716,44 +3720,44 @@
     <row r="69" ht="19.5" customHeight="1">
       <c r="A69" s="1" t="inlineStr">
         <is>
-          <t>rodinia_hybridsort</t>
+          <t>rodinia_lavaMD</t>
         </is>
       </c>
       <c r="B69" s="7" t="n">
         <v>0</v>
       </c>
       <c r="C69" s="7" t="n">
-        <v>106</v>
+        <v>46</v>
       </c>
       <c r="D69" s="7" t="n">
-        <v>84</v>
+        <v>20</v>
       </c>
       <c r="E69" s="7" t="n">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="F69" s="7" t="n">
-        <v>48</v>
+        <v>10</v>
       </c>
       <c r="G69" s="7" t="n">
-        <v>67</v>
+        <v>20</v>
       </c>
       <c r="H69" s="7" t="n">
-        <v>110</v>
+        <v>51</v>
       </c>
       <c r="I69" s="7" t="n">
-        <v>55</v>
+        <v>19</v>
       </c>
       <c r="J69" s="7" t="n">
-        <v>58</v>
+        <v>0</v>
       </c>
       <c r="K69" s="8" t="inlineStr">
         <is>
-          <t>0.2438150000</t>
+          <t>31.5730360000</t>
         </is>
       </c>
       <c r="L69" s="8" t="inlineStr">
         <is>
-          <t>0.3520820000</t>
+          <t>1.3297930000</t>
         </is>
       </c>
       <c r="M69" s="7" t="n"/>
@@ -3763,44 +3767,44 @@
     <row r="70" ht="19.5" customHeight="1">
       <c r="A70" s="1" t="inlineStr">
         <is>
-          <t>rodinia_lavaMD</t>
+          <t>rodinia_lud</t>
         </is>
       </c>
       <c r="B70" s="7" t="n">
         <v>0</v>
       </c>
       <c r="C70" s="7" t="n">
-        <v>46</v>
+        <v>440</v>
       </c>
       <c r="D70" s="7" t="n">
-        <v>20</v>
+        <v>186</v>
       </c>
       <c r="E70" s="7" t="n">
-        <v>17</v>
+        <v>44</v>
       </c>
       <c r="F70" s="7" t="n">
-        <v>10</v>
+        <v>291</v>
       </c>
       <c r="G70" s="7" t="n">
-        <v>20</v>
+        <v>44</v>
       </c>
       <c r="H70" s="7" t="n">
-        <v>51</v>
+        <v>572</v>
       </c>
       <c r="I70" s="7" t="n">
-        <v>19</v>
+        <v>42</v>
       </c>
       <c r="J70" s="7" t="n">
         <v>0</v>
       </c>
       <c r="K70" s="8" t="inlineStr">
         <is>
-          <t>31.5730360000</t>
+          <t>18.7550030000</t>
         </is>
       </c>
       <c r="L70" s="8" t="inlineStr">
         <is>
-          <t>1.3297930000</t>
+          <t>1.2440830000</t>
         </is>
       </c>
       <c r="M70" s="7" t="n"/>
@@ -3810,44 +3814,44 @@
     <row r="71" ht="19.5" customHeight="1">
       <c r="A71" s="1" t="inlineStr">
         <is>
-          <t>rodinia_lud</t>
+          <t>rodinia_myocyte</t>
         </is>
       </c>
       <c r="B71" s="7" t="n">
         <v>0</v>
       </c>
       <c r="C71" s="7" t="n">
-        <v>440</v>
+        <v>736</v>
       </c>
       <c r="D71" s="7" t="n">
-        <v>186</v>
+        <v>66</v>
       </c>
       <c r="E71" s="7" t="n">
-        <v>44</v>
+        <v>184</v>
       </c>
       <c r="F71" s="7" t="n">
-        <v>291</v>
+        <v>213</v>
       </c>
       <c r="G71" s="7" t="n">
-        <v>44</v>
+        <v>816</v>
       </c>
       <c r="H71" s="7" t="n">
-        <v>572</v>
+        <v>252</v>
       </c>
       <c r="I71" s="7" t="n">
-        <v>42</v>
+        <v>15</v>
       </c>
       <c r="J71" s="7" t="n">
         <v>0</v>
       </c>
       <c r="K71" s="8" t="inlineStr">
         <is>
-          <t>18.7550030000</t>
+          <t>1.7172340000</t>
         </is>
       </c>
       <c r="L71" s="8" t="inlineStr">
         <is>
-          <t>1.2440830000</t>
+          <t>2.9664410000</t>
         </is>
       </c>
       <c r="M71" s="7" t="n"/>
@@ -3857,44 +3861,44 @@
     <row r="72" ht="19.5" customHeight="1">
       <c r="A72" s="1" t="inlineStr">
         <is>
-          <t>rodinia_myocyte</t>
+          <t>rodinia_nn</t>
         </is>
       </c>
       <c r="B72" s="7" t="n">
         <v>0</v>
       </c>
       <c r="C72" s="7" t="n">
-        <v>736</v>
+        <v>9</v>
       </c>
       <c r="D72" s="7" t="n">
-        <v>66</v>
+        <v>7</v>
       </c>
       <c r="E72" s="7" t="n">
-        <v>184</v>
+        <v>5</v>
       </c>
       <c r="F72" s="7" t="n">
-        <v>213</v>
+        <v>1</v>
       </c>
       <c r="G72" s="7" t="n">
-        <v>816</v>
+        <v>5</v>
       </c>
       <c r="H72" s="7" t="n">
-        <v>252</v>
+        <v>6</v>
       </c>
       <c r="I72" s="7" t="n">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="J72" s="7" t="n">
         <v>0</v>
       </c>
       <c r="K72" s="8" t="inlineStr">
         <is>
-          <t>1.7172340000</t>
+          <t>0.0606480000</t>
         </is>
       </c>
       <c r="L72" s="8" t="inlineStr">
         <is>
-          <t>2.9664410000</t>
+          <t>0.0102400000</t>
         </is>
       </c>
       <c r="M72" s="7" t="n"/>
@@ -3904,29 +3908,29 @@
     <row r="73" ht="19.5" customHeight="1">
       <c r="A73" s="1" t="inlineStr">
         <is>
-          <t>rodinia_nn</t>
+          <t>rodinia_nw</t>
         </is>
       </c>
       <c r="B73" s="7" t="n">
         <v>0</v>
       </c>
       <c r="C73" s="7" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="D73" s="7" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E73" s="7" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F73" s="7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G73" s="7" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H73" s="7" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="I73" s="7" t="n">
         <v>4</v>
@@ -3936,12 +3940,12 @@
       </c>
       <c r="K73" s="8" t="inlineStr">
         <is>
-          <t>0.0606480000</t>
+          <t>0.4908550000</t>
         </is>
       </c>
       <c r="L73" s="8" t="inlineStr">
         <is>
-          <t>0.0102400000</t>
+          <t>0.9495210000</t>
         </is>
       </c>
       <c r="M73" s="7" t="n"/>
@@ -3951,44 +3955,44 @@
     <row r="74" ht="19.5" customHeight="1">
       <c r="A74" s="1" t="inlineStr">
         <is>
-          <t>rodinia_nw</t>
+          <t>rodinia_particlefilter_single</t>
         </is>
       </c>
       <c r="B74" s="7" t="n">
         <v>0</v>
       </c>
       <c r="C74" s="7" t="n">
-        <v>0</v>
+        <v>206</v>
       </c>
       <c r="D74" s="7" t="n">
-        <v>10</v>
+        <v>93</v>
       </c>
       <c r="E74" s="7" t="n">
-        <v>0</v>
+        <v>58</v>
       </c>
       <c r="F74" s="7" t="n">
-        <v>0</v>
+        <v>95</v>
       </c>
       <c r="G74" s="7" t="n">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="H74" s="7" t="n">
-        <v>0</v>
+        <v>158</v>
       </c>
       <c r="I74" s="7" t="n">
-        <v>4</v>
+        <v>93</v>
       </c>
       <c r="J74" s="7" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="K74" s="8" t="inlineStr">
         <is>
-          <t>0.4908550000</t>
+          <t>0.4632210000</t>
         </is>
       </c>
       <c r="L74" s="8" t="inlineStr">
         <is>
-          <t>0.9495210000</t>
+          <t>1.6567660000</t>
         </is>
       </c>
       <c r="M74" s="7" t="n"/>
@@ -3998,44 +4002,44 @@
     <row r="75" ht="19.5" customHeight="1">
       <c r="A75" s="1" t="inlineStr">
         <is>
-          <t>rodinia_particlefilter_single</t>
+          <t>rodinia_particlefilter_double</t>
         </is>
       </c>
       <c r="B75" s="7" t="n">
         <v>0</v>
       </c>
       <c r="C75" s="7" t="n">
-        <v>206</v>
+        <v>190</v>
       </c>
       <c r="D75" s="7" t="n">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="E75" s="7" t="n">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="F75" s="7" t="n">
-        <v>95</v>
+        <v>76</v>
       </c>
       <c r="G75" s="7" t="n">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="H75" s="7" t="n">
         <v>158</v>
       </c>
       <c r="I75" s="7" t="n">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="J75" s="7" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="K75" s="8" t="inlineStr">
         <is>
-          <t>0.4632210000</t>
+          <t>0.3353120000</t>
         </is>
       </c>
       <c r="L75" s="8" t="inlineStr">
         <is>
-          <t>1.6567660000</t>
+          <t>4.4983170000</t>
         </is>
       </c>
       <c r="M75" s="7" t="n"/>
@@ -4045,44 +4049,44 @@
     <row r="76" ht="19.5" customHeight="1">
       <c r="A76" s="1" t="inlineStr">
         <is>
-          <t>rodinia_particlefilter_double</t>
+          <t>rodinia_pathfinder</t>
         </is>
       </c>
       <c r="B76" s="7" t="n">
         <v>0</v>
       </c>
       <c r="C76" s="7" t="n">
-        <v>190</v>
+        <v>41</v>
       </c>
       <c r="D76" s="7" t="n">
-        <v>87</v>
+        <v>21</v>
       </c>
       <c r="E76" s="7" t="n">
-        <v>54</v>
+        <v>9</v>
       </c>
       <c r="F76" s="7" t="n">
-        <v>76</v>
+        <v>13</v>
       </c>
       <c r="G76" s="7" t="n">
-        <v>66</v>
+        <v>0</v>
       </c>
       <c r="H76" s="7" t="n">
-        <v>158</v>
+        <v>24</v>
       </c>
       <c r="I76" s="7" t="n">
-        <v>84</v>
+        <v>15</v>
       </c>
       <c r="J76" s="7" t="n">
         <v>0</v>
       </c>
       <c r="K76" s="8" t="inlineStr">
         <is>
-          <t>0.3353120000</t>
+          <t>1.1912450000</t>
         </is>
       </c>
       <c r="L76" s="8" t="inlineStr">
         <is>
-          <t>4.4983170000</t>
+          <t>0.1988960000</t>
         </is>
       </c>
       <c r="M76" s="7" t="n"/>
@@ -4092,40 +4096,44 @@
     <row r="77" ht="19.5" customHeight="1">
       <c r="A77" s="1" t="inlineStr">
         <is>
-          <t>rodinia_pathfinder</t>
+          <t>rodinia_streamcluster</t>
         </is>
       </c>
       <c r="B77" s="7" t="n">
         <v>0</v>
       </c>
       <c r="C77" s="7" t="n">
-        <v>41</v>
+        <v>55</v>
       </c>
       <c r="D77" s="7" t="n">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="E77" s="7" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F77" s="7" t="n">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="G77" s="7" t="n">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="H77" s="7" t="n">
-        <v>24</v>
+        <v>49</v>
       </c>
       <c r="I77" s="7" t="n">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="J77" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="K77" s="8" t="n"/>
+      <c r="K77" s="8" t="inlineStr">
+        <is>
+          <t>11.2296740000</t>
+        </is>
+      </c>
       <c r="L77" s="8" t="inlineStr">
         <is>
-          <t>0.1988960000</t>
+          <t>4.0395960000</t>
         </is>
       </c>
       <c r="M77" s="7" t="n"/>
@@ -4135,96 +4143,49 @@
     <row r="78" ht="19.5" customHeight="1">
       <c r="A78" s="1" t="inlineStr">
         <is>
-          <t>rodinia_streamcluster</t>
+          <t>rodinia_srad</t>
         </is>
       </c>
       <c r="B78" s="7" t="n">
         <v>0</v>
       </c>
       <c r="C78" s="7" t="n">
-        <v>55</v>
+        <v>131</v>
       </c>
       <c r="D78" s="7" t="n">
-        <v>29</v>
+        <v>58</v>
       </c>
       <c r="E78" s="7" t="n">
-        <v>11</v>
+        <v>31</v>
       </c>
       <c r="F78" s="7" t="n">
-        <v>19</v>
+        <v>68</v>
       </c>
       <c r="G78" s="7" t="n">
-        <v>12</v>
+        <v>47</v>
       </c>
       <c r="H78" s="7" t="n">
-        <v>49</v>
+        <v>128</v>
       </c>
       <c r="I78" s="7" t="n">
-        <v>19</v>
+        <v>48</v>
       </c>
       <c r="J78" s="7" t="n">
         <v>0</v>
       </c>
       <c r="K78" s="8" t="inlineStr">
         <is>
-          <t>11.2296740000</t>
+          <t>1.1714820000</t>
         </is>
       </c>
       <c r="L78" s="8" t="inlineStr">
         <is>
-          <t>4.0395960000</t>
+          <t>1.2007830000</t>
         </is>
       </c>
       <c r="M78" s="7" t="n"/>
       <c r="N78" s="13" t="n"/>
       <c r="O78" s="13" t="n"/>
-    </row>
-    <row r="79" ht="19.5" customHeight="1">
-      <c r="A79" s="1" t="inlineStr">
-        <is>
-          <t>rodinia_srad</t>
-        </is>
-      </c>
-      <c r="B79" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="C79" s="7" t="n">
-        <v>131</v>
-      </c>
-      <c r="D79" s="7" t="n">
-        <v>58</v>
-      </c>
-      <c r="E79" s="7" t="n">
-        <v>31</v>
-      </c>
-      <c r="F79" s="7" t="n">
-        <v>68</v>
-      </c>
-      <c r="G79" s="7" t="n">
-        <v>47</v>
-      </c>
-      <c r="H79" s="7" t="n">
-        <v>128</v>
-      </c>
-      <c r="I79" s="7" t="n">
-        <v>48</v>
-      </c>
-      <c r="J79" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="K79" s="8" t="inlineStr">
-        <is>
-          <t>1.1714820000</t>
-        </is>
-      </c>
-      <c r="L79" s="8" t="inlineStr">
-        <is>
-          <t>1.2007830000</t>
-        </is>
-      </c>
-      <c r="M79" s="7" t="n"/>
-      <c r="N79" s="13" t="n"/>
-      <c r="O79" s="13" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>